<commit_message>
Revert "replace xls file"
This reverts commit 4bcbe8dced5ed100a5cf7d5d7f6e4c91a722ced1.
</commit_message>
<xml_diff>
--- a/survey-resources/data-xls/demo-survey-v2.xlsx
+++ b/survey-resources/data-xls/demo-survey-v2.xlsx
@@ -1,94 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Siphachanh\05 USAID\NREL\2022-2024\Meeting_Workshop_Training\Task 02\OPENPATH commands translation\20230626\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AEA545-15F2-4C1A-B435-D0A76D3337C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>ST</author>
-  </authors>
-  <commentList>
-    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{CF7CA2E0-4FA4-4A06-A48C-34D4335D3210}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ST:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-I do not think it makesene for country context
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{9C9EB814-7973-4759-9F4D-0D7917B79B56}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ST:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">It is not make sene in terms of Lao context and based on local income, So, I would suggest to ask in Lao kip instead. 
-For example: less than 100 million LAK
-150 million to 250 million 
-250 million to 300 million 
-300 million to 350 million
-350 million to 400 million
-400 million or more
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="443">
   <si>
     <t>type</t>
   </si>
@@ -1417,355 +1345,13 @@
   </si>
   <si>
     <t>English (en)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label::ລາວ (lao) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hint::ລາວ (lao) </t>
-  </si>
-  <si>
-    <t>ເລີ້ມອອກເດີນທາງ</t>
-  </si>
-  <si>
-    <t>ສິ້ນສຸດການເດີນທາງ</t>
-  </si>
-  <si>
-    <t>ຂໍ້ມູນລະດັບຄົວເຮືອນ</t>
-  </si>
-  <si>
-    <t>label:: Lao (La)</t>
-  </si>
-  <si>
-    <t>ທ່ານມີຫຼາຍກວ່າໜຶ່ງວຽກບໍ?</t>
-  </si>
-  <si>
-    <t>ທ່ານ​ອາ​ຍຸ​ຈັກ​ປີ?</t>
-  </si>
-  <si>
-    <t>ທ່ານເປັນຄົນເຊື້ອຊາດ/ຊົນເຜົ່າໃດ?</t>
-  </si>
-  <si>
-    <t>ທ່ານມີໃບຂັບຂີ່ທີ່ບໍ?</t>
-  </si>
-  <si>
-    <t>ທ່ານ​ເປັນ​ນັກ​ສຶກສາ​ບໍ?</t>
-  </si>
-  <si>
-    <t>ລວມທັງຕົວທ່ານເອງ, ມີຈັກຄົນອາໄສຢູ່ໃນເຮືອນຂອງທ່ານ?</t>
-  </si>
-  <si>
-    <t>ລວມທັງຕົວທ່ານເອງ, ຄົນໃນເຮືອນຂອງທ່ານມີຈັກຄົນທີ່ເຮັດວຽກ?</t>
-  </si>
-  <si>
-    <t>ມີເດັກນ້ອຍອາຍຸຕ່ຳກວ່າ 18 ປີອາໄສຢູ່ໃນເຮືອນຂອງທ່ານຈັກຄົນ?</t>
-  </si>
-  <si>
-    <t>ທ່ານເປັນເຈົ້າຂອງລົດຈັກຄັນ ຫລື ເຊົ່າລົດຈັກຄັນ, ຄົນໃນເຮືອນຂອງທ່ານນໍາໃຊ້ລົດເປັນປົກກະຕິ?</t>
-  </si>
-  <si>
-    <t>ລວມທັງຕົວທ່ານເອງ, ຄົນໃນເຮືອນຂອງທ່ານມີຈັກຄົນທີ່ມີໃບຂັບຂີ່?</t>
-  </si>
-  <si>
-    <t>ຖ້າທ່ານບໍ່ສາມາດນໍາໃຊ້ພາຫະນະໃນເຮືອນຂອງທ່ານ (ຫຼືຖ້າບໍ່ມີທ່ານ), ທ່ານຈະເລືອກອັນໃດດັ່ງຕໍ່ໄປນີ້?</t>
-  </si>
-  <si>
-    <t>ທ່ານມີສະພາບທາງດ້ານຮ່າງກາຍ ທີ່ເຮັດໃຫ້ມັນມີຄວາມຫຍຸ້ງຍາກໃນການເດີນບໍ?</t>
-  </si>
-  <si>
-    <t>ທ່ານມີບັນຫາດ້ານຮ່າງກາຍດົນປານໃດ?</t>
-  </si>
-  <si>
-    <t>ຂໍ້ມູນທີ່ກ່ຽວຂ້ອງກັບວຽກຂອງທ່ານ</t>
-  </si>
-  <si>
-    <t>ທ່ານເຮັດວຽກເຕັມເວລາ ຫຼື ເຮັດວຽກລ່ວງເວລາ ບໍ?</t>
-  </si>
-  <si>
-    <t>ອັນໃດທີ່ບົ່ງບອກວ່າເປັນວຽກຫຼັກຂອງທ່ານ?</t>
-  </si>
-  <si>
-    <t>ຂໍໃຫ້ທ່ານໃຫ້ຂໍ້ມູນອັນທີ່ເປັນວຽກຫຼັກໆຂອງທ່ານ</t>
-  </si>
-  <si>
-    <t>ທ່ານມີຄວາມສາມາດໃນການກໍານົດຫຼືປ່ຽນເວລາເຂົ້າການດ້ວຍຕົວທ່ານເອງບໍ?</t>
-  </si>
-  <si>
-    <t>ທ່ານມີທາງເລືອກທີ່ຈະເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ໃດໜຶ່ງ ແທນທີ່ຈະເຂົ້າໄປເຮັດວຽກຢູ່ຫ້ອງການຂອງທ່ານ?</t>
-  </si>
-  <si>
-    <t>ປົກກະຕິມື້ໃດ ທີ່ທ່ານເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ອຶ່ນ ທີ່ບໍ່ແມ່ນຫ້ອງການຂອງທ່ານ</t>
-  </si>
-  <si>
-    <t>ປົກກະຕິຈັກວັນທ່ານເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ອຶ່ນ ທີ່ບໍ່ແມ່ນຫ້ອງການຂອງທ່ານ ຕໍ່ອາທິດ</t>
-  </si>
-  <si>
-    <t>ຂໍ້ມູນຂອງທ່ານ</t>
-  </si>
-  <si>
-    <t>ເພດຂອງທ່ານ?</t>
-  </si>
-  <si>
-    <t>ທ່ານຄິດວ່າທ່ານເອງເປັນ ຄົນຂ້າມເພດບໍ?</t>
-  </si>
-  <si>
-    <t>ຂໍ້ມູນໃດລຸ່ມນີ້ທີ່ກ່ຽວກັບທ່ານ?</t>
-  </si>
-  <si>
-    <t>ລະດັບການສຶກສາຂອງທ່ານ?</t>
-  </si>
-  <si>
-    <t>ທ່ານເປັນພະນັກງານບໍ?</t>
-  </si>
-  <si>
-    <t>ປະເພດເຮືອນຂອງທ່ານເປັນລັກສະນະແນວໃດ?</t>
-  </si>
-  <si>
-    <t>ທ່ານມີເຮືອນເປັນຂອງຕົນເອງບໍ ຫຼື ເຊົ່າເຮືອນເພີ່ນຢູ່?</t>
-  </si>
-  <si>
-    <t>ກະລຸນາເລືອກທັງໝົດ</t>
-  </si>
-  <si>
-    <t>ລວມທັງໂຮງຮຽນລັດ ແລະ ໂຮງຮຽນເອກະຊົນ ຫລື ຮຽນຢູ່ບ້ານ</t>
-  </si>
-  <si>
-    <t>ກະລຸນາລະບຸອັນໃດ ທີ່ເປັນລາຍຮັບຫຼັກໃນຄອບຂອງທ່ານ ສໍາລັບປີທີ່ຜ່ານມາ.</t>
-  </si>
-  <si>
-    <t>ເຫດຜົນທີ່ພວກເຮົາຖາມກ່ຽວກັບລາຍຮັບ ເນື່ອງຈາກເປັນພຽງການເກັບກໍາດ້ານສະຖິຕິ ໃນເວລາ ແລະ ວິທີການເດີນທາງ</t>
-  </si>
-  <si>
-    <t>ລວມທັງລົດຈັກ, ລົດຖີບທີ່ໃຊ້ມໍເຕີໄຟຟ້າ ແລະ ລົດບ້ານ</t>
-  </si>
-  <si>
-    <t>ພວກເຮົາໝາຍເຖີງ ເຮັດວຽກອຶ່ນນໍາ ເຊີ່ງີ່ມີຜູ້ທີ່ມາຈາ້ງທ່ານໃຫ້ເຮັດວຽກ (ທ່ານມີນາຍຈ້າງຫລາຍກ່ວາ 1)</t>
-  </si>
-  <si>
-    <t>ໃນເວລາທີ່ທ່ານເຮັດວຽກ ເຄີ່ງວັນ ຢູ່ເຮືອນ ຫລື ສະຖານທີ່ອຶ່ນ ແທນທີ່ບ່ອນເຮັດວຽກຂອງທ່ານ ແມ່ນຈະປັດໃຫ້ເປັນ 1 ວັນເລີຍ</t>
-  </si>
-  <si>
-    <t>16 ປີ ຫາ 20 ປີ</t>
-  </si>
-  <si>
-    <t>21 ປີ ຫາ 25 ປີ</t>
-  </si>
-  <si>
-    <t>26 ປີ ຫາ 30 ປີ</t>
-  </si>
-  <si>
-    <t>31 ປີ ຫາ 35 ປີ</t>
-  </si>
-  <si>
-    <t>36 ປີ ຫາ 40 ປີ</t>
-  </si>
-  <si>
-    <t>41 ປີ ຫາ 45 ປີ</t>
-  </si>
-  <si>
-    <t>46 ປີ ຫາ 50 ປີ</t>
-  </si>
-  <si>
-    <t>51 ປີ ຫາ 55 ປີ</t>
-  </si>
-  <si>
-    <t>56 ປີ ຫາ 60 ປີ</t>
-  </si>
-  <si>
-    <t>61 ປີ ຫາ 65 ປີ</t>
-  </si>
-  <si>
-    <t>ອາຍຸຕໍ່າກ່ວາ 16 ປີ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ອາຍຸຫລາຍກວ່າ 65 ປີ</t>
-  </si>
-  <si>
-    <t>ບໍ່ສະດວກໃຫ້ຂໍ້ມູນ</t>
-  </si>
-  <si>
-    <t>ເພດຊາຍ</t>
-  </si>
-  <si>
-    <t>ເພດຍິງ</t>
-  </si>
-  <si>
-    <t>ອຶ່ນໆ</t>
-  </si>
-  <si>
-    <t>ແມ່ນ</t>
-  </si>
-  <si>
-    <t>ບໍ່ແມ່ນ</t>
-  </si>
-  <si>
-    <t>ຄົນອາເມລິກາ ຜີວຂາວ</t>
-  </si>
-  <si>
-    <t>ຄົນອາເມລິກາ ຜີວດໍາ</t>
-  </si>
-  <si>
-    <t>ພາສາສະເປນ ຫລື ລາຕິນ</t>
-  </si>
-  <si>
-    <t>ອາຊີຕາເວັນອອກ</t>
-  </si>
-  <si>
-    <t>ອາຊີໄຕ້</t>
-  </si>
-  <si>
-    <t>ອິນເດຍ ອາເມລິກາ</t>
-  </si>
-  <si>
-    <t>ອາເມລິກາ ໃນໝູ່ເກາະຮາວາຍ</t>
-  </si>
-  <si>
-    <t>ຫລາຍເຊື້ອຊາດ</t>
-  </si>
-  <si>
-    <t>ບໍ່ແມ່ນ ນັກສຶກສາ</t>
-  </si>
-  <si>
-    <t>ແມ່ນ, ມັດທະຍົມສຶກສາ (ຕອນຕົ້ນ ແລະ ຕອນປາຍ)</t>
-  </si>
-  <si>
-    <t>ແມ່ນ, ການສຶກສາດ້ານວິຊາຊີບ</t>
-  </si>
-  <si>
-    <t>ແມ່ນ, ຮຽນເພີ້ມ ທີ່ວິທະຍາໄລ ຫລື ມະຫາວິທະຍາໄລ</t>
-  </si>
-  <si>
-    <t>ແມ່ນ, ຮຽນເຕັມເວລາ ທີ່ວິທະຍາໄລ ຫລື ມະຫາວິທະຍາໄລ</t>
-  </si>
-  <si>
-    <t>ຈົບການສຶກສາບໍ່ຮອດຂັ້ນມັດທະຍົມຕອນປາຍ</t>
-  </si>
-  <si>
-    <t>ຈົບການສຶກສາຊັ້ນສູງ</t>
-  </si>
-  <si>
-    <t>ຈົບການສຶກສາຂັ້ນມັດທະຍົມຕອນປາຍ</t>
-  </si>
-  <si>
-    <t>ຈົບການສຶກສາຂັ້ນ ປະລິນຍາຕີ</t>
-  </si>
-  <si>
-    <t>ຈົບການສຶກສາ ຂັ້ນປະລິນຍາໂທ ຫລື ສູງກ່ວາ</t>
-  </si>
-  <si>
-    <t>ຕອນນີ້ ຂ້ອຍຂາດວຽກຊົ່ວຄາວ</t>
-  </si>
-  <si>
-    <t>ຂ້ອຍບໍ່ສາມາດເຮັດວຽກໄດ້ ເນື່ອງຈາກສະພາບຮ່າງກາຍ, ກະສຽນແລ້ວ</t>
-  </si>
-  <si>
-    <t>ບໍ່ແມ່ນທັງໝົດ ຈາກຂ້າງເທີງ</t>
-  </si>
-  <si>
-    <t>ເປັນເຈົ້າຂອງເອງ</t>
-  </si>
-  <si>
-    <t>ເຊົ່າ</t>
-  </si>
-  <si>
-    <t>ບໍ່ແມ່ນທັງສອງ</t>
-  </si>
-  <si>
-    <t>ເຊົ່າອາຄານ ຫລື ເປັນອາພາດເມັນ</t>
-  </si>
-  <si>
-    <t>ສະເພາະຄອບຄົວເອງ</t>
-  </si>
-  <si>
-    <t>ມີຫລາຍຄອບຄົວອາໃສຢູ່ນໍາກັນ</t>
-  </si>
-  <si>
-    <t>ທີ່ລົບໄພ ຫລື ສະຖານທີ່ພັກຊົ່ວຄາວ</t>
-  </si>
-  <si>
-    <t>ຫລາຍກ່ວາ 7</t>
-  </si>
-  <si>
-    <t>ຫລາຍກ່ວາ 3</t>
-  </si>
-  <si>
-    <t>ຫລາຍກ່ວາ 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ການຂົນສົ່ງສາທາລະນະ (ລົດເມ, ລົດໄຟ) </t>
-  </si>
-  <si>
-    <t>ຂີ່ລົດໄປກັບໝູ່ ຫລື ຄົນໃນຄອບຄົວ ຫລື ໃນບ້ານດຽວກັນ</t>
-  </si>
-  <si>
-    <t>ເຊົ່າລົດ</t>
-  </si>
-  <si>
-    <t>ລົດຖີບ</t>
-  </si>
-  <si>
-    <t>ຍ່າງ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ແທັກຊີ </t>
-  </si>
-  <si>
-    <t>ບໍ່ມີ</t>
-  </si>
-  <si>
-    <t>6 ເດືອນ ຫລື ໜ້ອຍກ່ວາ</t>
-  </si>
-  <si>
-    <t>ຫລາຍກ່ວາ 6 ເດືອນ</t>
-  </si>
-  <si>
-    <t>ຕະຫລອດຊີວິດ</t>
-  </si>
-  <si>
-    <t>ເຕັມເວລາ</t>
-  </si>
-  <si>
-    <t>ລ່ວງເວລາ</t>
-  </si>
-  <si>
-    <t>ການຂາຍ ຫລື ວຽກບໍລິການ</t>
-  </si>
-  <si>
-    <t>ວຽກບໍລິຫານ</t>
-  </si>
-  <si>
-    <t>ວຽກໂຮງງານ, ການກໍໍ່ສ້າງ ຫລື ກະສິກໍາ</t>
-  </si>
-  <si>
-    <t>ວິຊາຊີບສະເພາະ, ການຈັດການ, ຫລື ເປັນຊ່າງຊໍານານງານສະເພາະດ້ານ</t>
-  </si>
-  <si>
-    <t>ວັນຈັນ</t>
-  </si>
-  <si>
-    <t>ວັນອັງຄານ</t>
-  </si>
-  <si>
-    <t>ວັນພຸດ</t>
-  </si>
-  <si>
-    <t>ວັນພະຫັດ</t>
-  </si>
-  <si>
-    <t>ວັນສຸກ</t>
-  </si>
-  <si>
-    <t>ວັນອາທິດ</t>
-  </si>
-  <si>
-    <t>ວັນເສົາ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1773,48 +1359,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Phetsarath OT"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Phet"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Saysettha OT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1829,37 +1380,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1897,7 +1432,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1931,7 +1466,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1966,10 +1500,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2142,26 +1675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
-  <cols>
-    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="105.44140625" customWidth="1"/>
-    <col min="5" max="5" width="65.5546875" customWidth="1"/>
-    <col min="6" max="6" width="50.21875" customWidth="1"/>
-    <col min="7" max="7" width="73.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="147.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2171,57 +1692,45 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>443</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>444</v>
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="22.8">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="22.8">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="22.8">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2231,17 +1740,14 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="22.8">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2251,17 +1757,14 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="22.8">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2271,17 +1774,14 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="G6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="22.8">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2291,20 +1791,17 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="22.8">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2314,26 +1811,20 @@
       <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>451</v>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="H8" t="s">
         <v>36</v>
       </c>
-      <c r="I8" t="s">
+      <c r="G8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="22.8">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2343,17 +1834,14 @@
       <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="I9" t="s">
+      <c r="G9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="22.8">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2363,26 +1851,20 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>453</v>
+      <c r="D10" t="s">
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="H10" t="s">
         <v>46</v>
       </c>
-      <c r="I10" t="s">
+      <c r="G10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="22.8">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2392,17 +1874,14 @@
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="I11" t="s">
+      <c r="G11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="22.8">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2412,17 +1891,14 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="I12" t="s">
+      <c r="G12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="22.8">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2432,26 +1908,22 @@
       <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
       <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="22.8">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="22.8">
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2461,17 +1933,14 @@
       <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
         <v>63</v>
       </c>
-      <c r="I15" t="s">
+      <c r="G15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="22.8">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2481,17 +1950,14 @@
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
         <v>67</v>
       </c>
-      <c r="I16" t="s">
+      <c r="G16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="22.8">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2501,17 +1967,14 @@
       <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="I17" t="s">
+      <c r="G17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="22.8">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2521,26 +1984,20 @@
       <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>480</v>
+      <c r="D18" t="s">
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="H18" t="s">
         <v>77</v>
       </c>
-      <c r="I18" t="s">
+      <c r="G18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22.8">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -2550,17 +2007,14 @@
       <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
         <v>81</v>
       </c>
-      <c r="I19" t="s">
+      <c r="G19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="22.8">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2570,17 +2024,14 @@
       <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>85</v>
       </c>
-      <c r="I20" t="s">
+      <c r="G20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="22.8">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2590,17 +2041,14 @@
       <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" t="s">
         <v>88</v>
       </c>
-      <c r="I21" t="s">
+      <c r="G21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="22.8">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -2610,17 +2058,14 @@
       <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
         <v>92</v>
       </c>
-      <c r="I22" t="s">
+      <c r="G22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="22.8">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2630,26 +2075,20 @@
       <c r="C23" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>457</v>
+      <c r="D23" t="s">
+        <v>96</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="H23" t="s">
         <v>98</v>
       </c>
-      <c r="I23" t="s">
+      <c r="G23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="22.8">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2659,17 +2098,14 @@
       <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>102</v>
       </c>
-      <c r="I24" t="s">
+      <c r="G24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="22.8">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -2679,17 +2115,14 @@
       <c r="C25" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>106</v>
       </c>
-      <c r="I25" t="s">
+      <c r="G25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="22.8">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -2699,26 +2132,22 @@
       <c r="C26" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
         <v>110</v>
       </c>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
       <c r="I26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="22.8">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" ht="22.8">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2728,20 +2157,17 @@
       <c r="C28" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s">
         <v>114</v>
       </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
       <c r="I28" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="22.8">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -2751,26 +2177,20 @@
       <c r="C29" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>449</v>
+      <c r="D29" t="s">
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="H29" t="s">
         <v>121</v>
       </c>
-      <c r="I29" t="s">
+      <c r="G29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="22.8">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -2780,23 +2200,20 @@
       <c r="C30" t="s">
         <v>124</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>463</v>
+      <c r="D30" t="s">
+        <v>125</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>126</v>
-      </c>
-      <c r="H30" t="s">
         <v>127</v>
       </c>
-      <c r="I30" t="s">
+      <c r="G30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="22.8">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -2806,17 +2223,14 @@
       <c r="C31" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" t="s">
         <v>131</v>
       </c>
-      <c r="I31" t="s">
+      <c r="G31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="22.8">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>132</v>
       </c>
@@ -2826,26 +2240,23 @@
       <c r="C32" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>465</v>
+      <c r="D32" t="s">
+        <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F32" t="s">
-        <v>136</v>
-      </c>
-      <c r="H32" t="s">
         <v>137</v>
       </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
       <c r="I32" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="22.8">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -2855,17 +2266,14 @@
       <c r="C33" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D33" t="s">
         <v>142</v>
       </c>
-      <c r="I33" t="s">
+      <c r="G33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="22.8">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -2875,17 +2283,14 @@
       <c r="C34" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D34" t="s">
         <v>146</v>
       </c>
-      <c r="I34" t="s">
+      <c r="G34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="22.8">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -2895,29 +2300,23 @@
       <c r="C35" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>469</v>
+      <c r="D35" t="s">
+        <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F35" t="s">
-        <v>151</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="H35" t="s">
         <v>152</v>
       </c>
+      <c r="G35" t="s">
+        <v>21</v>
+      </c>
       <c r="I35" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="22.8">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -2927,79 +2326,52 @@
       <c r="C36" t="s">
         <v>156</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>468</v>
+      <c r="D36" t="s">
+        <v>157</v>
       </c>
       <c r="E36" t="s">
-        <v>157</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="H36" t="s">
         <v>36</v>
       </c>
+      <c r="G36" t="s">
+        <v>21</v>
+      </c>
       <c r="I36" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="22.8">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" ht="22.8">
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>159</v>
       </c>
       <c r="B38" t="s">
         <v>160</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="L38" t="s">
+      <c r="J38" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="D40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="12" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <customProperties>
-    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="68.88671875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>162</v>
       </c>
@@ -3009,17 +2381,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>448</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>164</v>
       </c>
@@ -3029,14 +2398,11 @@
       <c r="C2" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -3046,14 +2412,11 @@
       <c r="C3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3063,14 +2426,11 @@
       <c r="C4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -3080,14 +2440,11 @@
       <c r="C5" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -3097,14 +2454,11 @@
       <c r="C6" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -3114,14 +2468,11 @@
       <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -3131,14 +2482,11 @@
       <c r="C8" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -3148,14 +2496,11 @@
       <c r="C9" t="s">
         <v>187</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -3165,14 +2510,11 @@
       <c r="C10" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -3182,14 +2524,11 @@
       <c r="C11" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -3199,14 +2538,11 @@
       <c r="C12" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -3216,14 +2552,11 @@
       <c r="C13" t="s">
         <v>199</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -3233,14 +2566,11 @@
       <c r="C14" t="s">
         <v>202</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -3250,14 +2580,11 @@
       <c r="C15" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -3267,14 +2594,11 @@
       <c r="C16" t="s">
         <v>209</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -3284,14 +2608,11 @@
       <c r="C17" t="s">
         <v>212</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>204</v>
       </c>
@@ -3301,14 +2622,11 @@
       <c r="C18" t="s">
         <v>215</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -3318,14 +2636,11 @@
       <c r="C19" t="s">
         <v>202</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D19" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -3335,14 +2650,11 @@
       <c r="C20" t="s">
         <v>219</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>217</v>
       </c>
@@ -3352,14 +2664,11 @@
       <c r="C21" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>217</v>
       </c>
@@ -3369,65 +2678,53 @@
       <c r="C22" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>222</v>
       </c>
       <c r="B23" t="s">
         <v>223</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>224</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>222</v>
       </c>
       <c r="B24" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s">
         <v>227</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>222</v>
       </c>
       <c r="B25" t="s">
         <v>229</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s">
         <v>230</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>222</v>
       </c>
@@ -3437,14 +2734,11 @@
       <c r="C26" t="s">
         <v>233</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>222</v>
       </c>
@@ -3454,14 +2748,11 @@
       <c r="C27" t="s">
         <v>236</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>222</v>
       </c>
@@ -3471,14 +2762,11 @@
       <c r="C28" t="s">
         <v>239</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>222</v>
       </c>
@@ -3488,14 +2776,11 @@
       <c r="C29" t="s">
         <v>242</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D29" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>222</v>
       </c>
@@ -3505,14 +2790,11 @@
       <c r="C30" t="s">
         <v>245</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>222</v>
       </c>
@@ -3522,14 +2804,11 @@
       <c r="C31" t="s">
         <v>215</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D31" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>222</v>
       </c>
@@ -3539,14 +2818,11 @@
       <c r="C32" t="s">
         <v>202</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -3556,14 +2832,11 @@
       <c r="C33" t="s">
         <v>219</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D33" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -3573,14 +2846,11 @@
       <c r="C34" t="s">
         <v>221</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D34" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -3590,14 +2860,11 @@
       <c r="C35" t="s">
         <v>202</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>249</v>
       </c>
@@ -3607,14 +2874,11 @@
       <c r="C36" t="s">
         <v>251</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>249</v>
       </c>
@@ -3624,14 +2888,11 @@
       <c r="C37" t="s">
         <v>254</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D37" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>249</v>
       </c>
@@ -3641,14 +2902,11 @@
       <c r="C38" t="s">
         <v>257</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>249</v>
       </c>
@@ -3658,14 +2916,11 @@
       <c r="C39" t="s">
         <v>260</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>249</v>
       </c>
@@ -3675,14 +2930,11 @@
       <c r="C40" t="s">
         <v>263</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>249</v>
       </c>
@@ -3692,14 +2944,11 @@
       <c r="C41" t="s">
         <v>202</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>265</v>
       </c>
@@ -3709,14 +2958,11 @@
       <c r="C42" t="s">
         <v>267</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D42" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>265</v>
       </c>
@@ -3726,14 +2972,11 @@
       <c r="C43" t="s">
         <v>270</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>265</v>
       </c>
@@ -3743,14 +2986,11 @@
       <c r="C44" t="s">
         <v>273</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D44" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>265</v>
       </c>
@@ -3760,14 +3000,11 @@
       <c r="C45" t="s">
         <v>276</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D45" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>265</v>
       </c>
@@ -3777,14 +3014,11 @@
       <c r="C46" t="s">
         <v>279</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D46" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>265</v>
       </c>
@@ -3794,14 +3028,11 @@
       <c r="C47" t="s">
         <v>202</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>281</v>
       </c>
@@ -3811,14 +3042,11 @@
       <c r="C48" t="s">
         <v>219</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D48" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>281</v>
       </c>
@@ -3828,14 +3056,11 @@
       <c r="C49" t="s">
         <v>221</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>281</v>
       </c>
@@ -3845,14 +3070,11 @@
       <c r="C50" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="D50" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>283</v>
       </c>
@@ -3862,14 +3084,11 @@
       <c r="C51" t="s">
         <v>285</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="D51" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>283</v>
       </c>
@@ -3879,17 +3098,14 @@
       <c r="C52" t="s">
         <v>288</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" t="s">
         <v>289</v>
       </c>
-      <c r="F52">
+      <c r="E52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -3899,17 +3115,14 @@
       <c r="C53" t="s">
         <v>291</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" t="s">
         <v>292</v>
       </c>
-      <c r="F53">
+      <c r="E53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>283</v>
       </c>
@@ -3919,17 +3132,14 @@
       <c r="C54" t="s">
         <v>202</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="D54" t="s">
         <v>203</v>
       </c>
-      <c r="F54">
+      <c r="E54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>293</v>
       </c>
@@ -3939,14 +3149,11 @@
       <c r="C55" t="s">
         <v>295</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>293</v>
       </c>
@@ -3956,17 +3163,14 @@
       <c r="C56" t="s">
         <v>298</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D56" t="s">
         <v>299</v>
       </c>
-      <c r="F56">
+      <c r="E56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>293</v>
       </c>
@@ -3976,17 +3180,14 @@
       <c r="C57" t="s">
         <v>301</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="D57" t="s">
         <v>302</v>
       </c>
-      <c r="F57">
+      <c r="E57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>293</v>
       </c>
@@ -3996,17 +3197,14 @@
       <c r="C58" t="s">
         <v>202</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D58" t="s">
         <v>203</v>
       </c>
-      <c r="F58">
+      <c r="E58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>303</v>
       </c>
@@ -4016,14 +3214,11 @@
       <c r="C59" t="s">
         <v>305</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D59" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>303</v>
       </c>
@@ -4033,17 +3228,14 @@
       <c r="C60" t="s">
         <v>308</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D60" t="s">
         <v>309</v>
       </c>
-      <c r="F60">
+      <c r="E60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>303</v>
       </c>
@@ -4053,17 +3245,14 @@
       <c r="C61" t="s">
         <v>311</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="D61" t="s">
         <v>312</v>
       </c>
-      <c r="F61">
+      <c r="E61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -4073,17 +3262,14 @@
       <c r="C62" t="s">
         <v>314</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="D62" t="s">
         <v>315</v>
       </c>
-      <c r="F62">
+      <c r="E62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>303</v>
       </c>
@@ -4093,101 +3279,98 @@
       <c r="C63" t="s">
         <v>202</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D63" t="s">
         <v>203</v>
       </c>
-      <c r="F63">
+      <c r="E63">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>316</v>
       </c>
       <c r="B64" t="s">
         <v>317</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" t="s">
         <v>318</v>
       </c>
-      <c r="E64" t="s">
+      <c r="D64" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>316</v>
       </c>
       <c r="B65" t="s">
         <v>320</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" t="s">
         <v>321</v>
       </c>
-      <c r="E65" t="s">
+      <c r="D65" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>316</v>
       </c>
       <c r="B66" t="s">
         <v>323</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" t="s">
         <v>324</v>
       </c>
-      <c r="E66" t="s">
+      <c r="D66" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>316</v>
       </c>
       <c r="B67" t="s">
         <v>326</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" t="s">
         <v>327</v>
       </c>
-      <c r="E67" t="s">
+      <c r="D67" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>316</v>
       </c>
       <c r="B68" t="s">
         <v>329</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" t="s">
         <v>330</v>
       </c>
-      <c r="E68" t="s">
+      <c r="D68" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>316</v>
       </c>
       <c r="B69" t="s">
         <v>332</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" t="s">
         <v>333</v>
       </c>
-      <c r="E69" t="s">
+      <c r="D69" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>316</v>
       </c>
@@ -4197,14 +3380,11 @@
       <c r="C70" t="s">
         <v>202</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="D70" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>335</v>
       </c>
@@ -4214,14 +3394,11 @@
       <c r="C71" t="s">
         <v>336</v>
       </c>
-      <c r="D71" s="5">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D71" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>335</v>
       </c>
@@ -4231,14 +3408,11 @@
       <c r="C72" t="s">
         <v>337</v>
       </c>
-      <c r="D72" s="5">
-        <v>2</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="D72" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>335</v>
       </c>
@@ -4248,14 +3422,11 @@
       <c r="C73" t="s">
         <v>338</v>
       </c>
-      <c r="D73" s="5">
-        <v>3</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="D73" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>335</v>
       </c>
@@ -4265,14 +3436,11 @@
       <c r="C74" t="s">
         <v>339</v>
       </c>
-      <c r="D74" s="5">
-        <v>4</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="D74" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>335</v>
       </c>
@@ -4282,14 +3450,11 @@
       <c r="C75" t="s">
         <v>340</v>
       </c>
-      <c r="D75" s="5">
-        <v>5</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="D75" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>335</v>
       </c>
@@ -4299,14 +3464,11 @@
       <c r="C76" t="s">
         <v>341</v>
       </c>
-      <c r="D76" s="5">
-        <v>6</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="D76" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>335</v>
       </c>
@@ -4316,14 +3478,11 @@
       <c r="C77" t="s">
         <v>342</v>
       </c>
-      <c r="D77" s="5">
-        <v>7</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="D77" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>335</v>
       </c>
@@ -4333,14 +3492,11 @@
       <c r="C78" t="s">
         <v>344</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="D78" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>335</v>
       </c>
@@ -4350,14 +3506,11 @@
       <c r="C79" t="s">
         <v>202</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="D79" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>346</v>
       </c>
@@ -4367,14 +3520,11 @@
       <c r="C80" t="s">
         <v>347</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D80" t="s">
         <v>347</v>
       </c>
-      <c r="E80" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>346</v>
       </c>
@@ -4384,17 +3534,14 @@
       <c r="C81" t="s">
         <v>336</v>
       </c>
-      <c r="D81" s="5">
-        <v>1</v>
+      <c r="D81" t="s">
+        <v>336</v>
       </c>
       <c r="E81" t="s">
         <v>336</v>
       </c>
-      <c r="F81" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>346</v>
       </c>
@@ -4404,17 +3551,14 @@
       <c r="C82" t="s">
         <v>337</v>
       </c>
-      <c r="D82" s="5">
-        <v>2</v>
+      <c r="D82" t="s">
+        <v>337</v>
       </c>
       <c r="E82" t="s">
         <v>337</v>
       </c>
-      <c r="F82" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -4424,17 +3568,14 @@
       <c r="C83" t="s">
         <v>338</v>
       </c>
-      <c r="D83" s="5">
-        <v>3</v>
+      <c r="D83" t="s">
+        <v>338</v>
       </c>
       <c r="E83" t="s">
         <v>338</v>
       </c>
-      <c r="F83" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>346</v>
       </c>
@@ -4444,17 +3585,14 @@
       <c r="C84" t="s">
         <v>339</v>
       </c>
-      <c r="D84" s="5">
-        <v>4</v>
+      <c r="D84" t="s">
+        <v>339</v>
       </c>
       <c r="E84" t="s">
         <v>339</v>
       </c>
-      <c r="F84" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>346</v>
       </c>
@@ -4464,17 +3602,14 @@
       <c r="C85" t="s">
         <v>349</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>533</v>
+      <c r="D85" t="s">
+        <v>350</v>
       </c>
       <c r="E85" t="s">
-        <v>350</v>
-      </c>
-      <c r="F85" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>346</v>
       </c>
@@ -4484,17 +3619,14 @@
       <c r="C86" t="s">
         <v>202</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>497</v>
+      <c r="D86" t="s">
+        <v>203</v>
       </c>
       <c r="E86" t="s">
-        <v>203</v>
-      </c>
-      <c r="F86" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>351</v>
       </c>
@@ -4504,14 +3636,11 @@
       <c r="C87" t="s">
         <v>347</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" t="s">
         <v>347</v>
       </c>
-      <c r="E87" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>351</v>
       </c>
@@ -4521,14 +3650,11 @@
       <c r="C88" t="s">
         <v>336</v>
       </c>
-      <c r="D88" s="5">
-        <v>1</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="D88" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>351</v>
       </c>
@@ -4538,14 +3664,11 @@
       <c r="C89" t="s">
         <v>337</v>
       </c>
-      <c r="D89" s="5">
-        <v>2</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="D89" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>351</v>
       </c>
@@ -4555,14 +3678,11 @@
       <c r="C90" t="s">
         <v>338</v>
       </c>
-      <c r="D90" s="5">
-        <v>3</v>
-      </c>
-      <c r="E90" t="s">
+      <c r="D90" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>351</v>
       </c>
@@ -4572,14 +3692,11 @@
       <c r="C91" t="s">
         <v>339</v>
       </c>
-      <c r="D91" s="5">
-        <v>4</v>
-      </c>
-      <c r="E91" t="s">
+      <c r="D91" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>351</v>
       </c>
@@ -4589,14 +3706,11 @@
       <c r="C92" t="s">
         <v>349</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="D92" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>351</v>
       </c>
@@ -4606,14 +3720,11 @@
       <c r="C93" t="s">
         <v>202</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E93" t="s">
+      <c r="D93" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>352</v>
       </c>
@@ -4623,14 +3734,11 @@
       <c r="C94" t="s">
         <v>347</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D94" t="s">
         <v>347</v>
       </c>
-      <c r="E94" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>352</v>
       </c>
@@ -4640,14 +3748,11 @@
       <c r="C95" t="s">
         <v>336</v>
       </c>
-      <c r="D95" s="5">
-        <v>1</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="D95" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>352</v>
       </c>
@@ -4657,14 +3762,11 @@
       <c r="C96" t="s">
         <v>337</v>
       </c>
-      <c r="D96" s="5">
-        <v>2</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="D96" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>352</v>
       </c>
@@ -4674,14 +3776,11 @@
       <c r="C97" t="s">
         <v>338</v>
       </c>
-      <c r="D97" s="5">
-        <v>3</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="D97" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>352</v>
       </c>
@@ -4691,14 +3790,11 @@
       <c r="C98" t="s">
         <v>354</v>
       </c>
-      <c r="D98" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="D98" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>352</v>
       </c>
@@ -4708,14 +3804,11 @@
       <c r="C99" t="s">
         <v>202</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="D99" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>356</v>
       </c>
@@ -4725,14 +3818,11 @@
       <c r="C100" t="s">
         <v>358</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="D100" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>356</v>
       </c>
@@ -4742,14 +3832,11 @@
       <c r="C101" t="s">
         <v>361</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="D101" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>356</v>
       </c>
@@ -4759,14 +3846,11 @@
       <c r="C102" t="s">
         <v>364</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="D102" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>356</v>
       </c>
@@ -4776,14 +3860,11 @@
       <c r="C103" t="s">
         <v>367</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D103" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>356</v>
       </c>
@@ -4793,14 +3874,11 @@
       <c r="C104" t="s">
         <v>370</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="D104" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>356</v>
       </c>
@@ -4810,14 +3888,11 @@
       <c r="C105" t="s">
         <v>373</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="D105" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>356</v>
       </c>
@@ -4827,14 +3902,11 @@
       <c r="C106" t="s">
         <v>376</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="D106" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>356</v>
       </c>
@@ -4844,14 +3916,11 @@
       <c r="C107" t="s">
         <v>202</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="D107" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>377</v>
       </c>
@@ -4861,14 +3930,11 @@
       <c r="C108" t="s">
         <v>219</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="D108" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>377</v>
       </c>
@@ -4878,14 +3944,11 @@
       <c r="C109" t="s">
         <v>221</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="D109" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>377</v>
       </c>
@@ -4895,14 +3958,11 @@
       <c r="C110" t="s">
         <v>202</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="D110" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>378</v>
       </c>
@@ -4912,14 +3972,11 @@
       <c r="C111" t="s">
         <v>380</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="D111" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>378</v>
       </c>
@@ -4929,14 +3986,11 @@
       <c r="C112" t="s">
         <v>383</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="D112" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -4946,14 +4000,11 @@
       <c r="C113" t="s">
         <v>386</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="E113" t="s">
+      <c r="D113" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>378</v>
       </c>
@@ -4963,14 +4014,11 @@
       <c r="C114" t="s">
         <v>202</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D114" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>389</v>
       </c>
@@ -4980,14 +4028,11 @@
       <c r="C115" t="s">
         <v>219</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="D115" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>389</v>
       </c>
@@ -4997,14 +4042,11 @@
       <c r="C116" t="s">
         <v>221</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="D116" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>389</v>
       </c>
@@ -5014,14 +4056,11 @@
       <c r="C117" t="s">
         <v>202</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E117" t="s">
+      <c r="D117" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>390</v>
       </c>
@@ -5031,14 +4070,11 @@
       <c r="C118" t="s">
         <v>392</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="E118" t="s">
+      <c r="D118" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>390</v>
       </c>
@@ -5048,14 +4084,11 @@
       <c r="C119" t="s">
         <v>395</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="E119" t="s">
+      <c r="D119" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>390</v>
       </c>
@@ -5065,14 +4098,11 @@
       <c r="C120" t="s">
         <v>202</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E120" t="s">
+      <c r="D120" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>397</v>
       </c>
@@ -5082,14 +4112,11 @@
       <c r="C121" t="s">
         <v>399</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="D121" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>397</v>
       </c>
@@ -5099,14 +4126,11 @@
       <c r="C122" t="s">
         <v>402</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="E122" t="s">
+      <c r="D122" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>397</v>
       </c>
@@ -5116,14 +4140,11 @@
       <c r="C123" t="s">
         <v>405</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="E123" t="s">
+      <c r="D123" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>397</v>
       </c>
@@ -5133,14 +4154,11 @@
       <c r="C124" t="s">
         <v>408</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="E124" t="s">
+      <c r="D124" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>397</v>
       </c>
@@ -5150,14 +4168,11 @@
       <c r="C125" t="s">
         <v>215</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E125" t="s">
+      <c r="D125" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>397</v>
       </c>
@@ -5167,14 +4182,11 @@
       <c r="C126" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="D126" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>410</v>
       </c>
@@ -5184,14 +4196,11 @@
       <c r="C127" t="s">
         <v>219</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="D127" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -5201,14 +4210,11 @@
       <c r="C128" t="s">
         <v>221</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D128" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>410</v>
       </c>
@@ -5218,14 +4224,11 @@
       <c r="C129" t="s">
         <v>202</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E129" t="s">
+      <c r="D129" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>411</v>
       </c>
@@ -5235,14 +4238,11 @@
       <c r="C130" t="s">
         <v>219</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="D130" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>411</v>
       </c>
@@ -5252,14 +4252,11 @@
       <c r="C131" t="s">
         <v>221</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="D131" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>411</v>
       </c>
@@ -5269,14 +4266,11 @@
       <c r="C132" t="s">
         <v>202</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="D132" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>412</v>
       </c>
@@ -5286,14 +4280,11 @@
       <c r="C133" t="s">
         <v>347</v>
       </c>
-      <c r="D133" s="6" t="s">
+      <c r="D133" t="s">
         <v>347</v>
       </c>
-      <c r="E133" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>412</v>
       </c>
@@ -5303,14 +4294,11 @@
       <c r="C134" t="s">
         <v>336</v>
       </c>
-      <c r="D134" s="5">
-        <v>1</v>
-      </c>
-      <c r="E134" t="s">
+      <c r="D134" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>412</v>
       </c>
@@ -5320,14 +4308,11 @@
       <c r="C135" t="s">
         <v>337</v>
       </c>
-      <c r="D135" s="5">
-        <v>2</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="D135" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>412</v>
       </c>
@@ -5337,14 +4322,11 @@
       <c r="C136" t="s">
         <v>338</v>
       </c>
-      <c r="D136" s="5">
-        <v>3</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="D136" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>412</v>
       </c>
@@ -5354,14 +4336,11 @@
       <c r="C137" t="s">
         <v>339</v>
       </c>
-      <c r="D137" s="5">
-        <v>4</v>
-      </c>
-      <c r="E137" t="s">
+      <c r="D137" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>412</v>
       </c>
@@ -5371,14 +4350,11 @@
       <c r="C138" t="s">
         <v>340</v>
       </c>
-      <c r="D138" s="5">
-        <v>5</v>
-      </c>
-      <c r="E138" t="s">
+      <c r="D138" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>412</v>
       </c>
@@ -5388,14 +4364,11 @@
       <c r="C139" t="s">
         <v>341</v>
       </c>
-      <c r="D139" s="5">
-        <v>6</v>
-      </c>
-      <c r="E139" t="s">
+      <c r="D139" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>412</v>
       </c>
@@ -5405,14 +4378,11 @@
       <c r="C140" t="s">
         <v>342</v>
       </c>
-      <c r="D140" s="5">
-        <v>7</v>
-      </c>
-      <c r="E140" t="s">
+      <c r="D140" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>412</v>
       </c>
@@ -5422,14 +4392,11 @@
       <c r="C141" t="s">
         <v>202</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E141" t="s">
+      <c r="D141" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>413</v>
       </c>
@@ -5439,14 +4406,11 @@
       <c r="C142" t="s">
         <v>415</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="E142" t="s">
+      <c r="D142" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>413</v>
       </c>
@@ -5456,14 +4420,11 @@
       <c r="C143" t="s">
         <v>418</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="E143" t="s">
+      <c r="D143" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>413</v>
       </c>
@@ -5473,14 +4434,11 @@
       <c r="C144" t="s">
         <v>421</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E144" t="s">
+      <c r="D144" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>413</v>
       </c>
@@ -5490,14 +4448,11 @@
       <c r="C145" t="s">
         <v>424</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E145" t="s">
+      <c r="D145" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>413</v>
       </c>
@@ -5507,14 +4462,11 @@
       <c r="C146" t="s">
         <v>427</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="E146" t="s">
+      <c r="D146" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>413</v>
       </c>
@@ -5524,14 +4476,11 @@
       <c r="C147" t="s">
         <v>430</v>
       </c>
-      <c r="D147" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="E147" t="s">
+      <c r="D147" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>413</v>
       </c>
@@ -5541,14 +4490,11 @@
       <c r="C148" t="s">
         <v>433</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="E148" t="s">
+      <c r="D148" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>413</v>
       </c>
@@ -5558,29 +4504,22 @@
       <c r="C149" t="s">
         <v>202</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E149" t="s">
+      <c r="D149" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId1"/>
-  </customProperties>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -5612,8 +4551,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId1"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Lao to survey (#999)
* replace file w/ Lao translations included

replaced survey file with one that includes Lao translations

* Update demo-survey-v2.xml

* replace xls file

* Revert "replace xls file"

This reverts commit 4bcbe8dced5ed100a5cf7d5d7f6e4c91a722ced1.

* replace xls file

* replace json file with additional language
</commit_message>
<xml_diff>
--- a/survey-resources/data-xls/demo-survey-v2.xlsx
+++ b/survey-resources/data-xls/demo-survey-v2.xlsx
@@ -1,22 +1,94 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Siphachanh\05 USAID\NREL\2022-2024\Meeting_Workshop_Training\Task 02\OPENPATH commands translation\20230626\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AEA545-15F2-4C1A-B435-D0A76D3337C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ST</author>
+  </authors>
+  <commentList>
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{CF7CA2E0-4FA4-4A06-A48C-34D4335D3210}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ST:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I do not think it makesene for country context
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{9C9EB814-7973-4759-9F4D-0D7917B79B56}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ST:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">It is not make sene in terms of Lao context and based on local income, So, I would suggest to ask in Lao kip instead. 
+For example: less than 100 million LAK
+150 million to 250 million 
+250 million to 300 million 
+300 million to 350 million
+350 million to 400 million
+400 million or more
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="557">
   <si>
     <t>type</t>
   </si>
@@ -1345,13 +1417,355 @@
   </si>
   <si>
     <t>English (en)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label::ລາວ (lao) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint::ລາວ (lao) </t>
+  </si>
+  <si>
+    <t>ເລີ້ມອອກເດີນທາງ</t>
+  </si>
+  <si>
+    <t>ສິ້ນສຸດການເດີນທາງ</t>
+  </si>
+  <si>
+    <t>ຂໍ້ມູນລະດັບຄົວເຮືອນ</t>
+  </si>
+  <si>
+    <t>label:: Lao (La)</t>
+  </si>
+  <si>
+    <t>ທ່ານມີຫຼາຍກວ່າໜຶ່ງວຽກບໍ?</t>
+  </si>
+  <si>
+    <t>ທ່ານ​ອາ​ຍຸ​ຈັກ​ປີ?</t>
+  </si>
+  <si>
+    <t>ທ່ານເປັນຄົນເຊື້ອຊາດ/ຊົນເຜົ່າໃດ?</t>
+  </si>
+  <si>
+    <t>ທ່ານມີໃບຂັບຂີ່ທີ່ບໍ?</t>
+  </si>
+  <si>
+    <t>ທ່ານ​ເປັນ​ນັກ​ສຶກສາ​ບໍ?</t>
+  </si>
+  <si>
+    <t>ລວມທັງຕົວທ່ານເອງ, ມີຈັກຄົນອາໄສຢູ່ໃນເຮືອນຂອງທ່ານ?</t>
+  </si>
+  <si>
+    <t>ລວມທັງຕົວທ່ານເອງ, ຄົນໃນເຮືອນຂອງທ່ານມີຈັກຄົນທີ່ເຮັດວຽກ?</t>
+  </si>
+  <si>
+    <t>ມີເດັກນ້ອຍອາຍຸຕ່ຳກວ່າ 18 ປີອາໄສຢູ່ໃນເຮືອນຂອງທ່ານຈັກຄົນ?</t>
+  </si>
+  <si>
+    <t>ທ່ານເປັນເຈົ້າຂອງລົດຈັກຄັນ ຫລື ເຊົ່າລົດຈັກຄັນ, ຄົນໃນເຮືອນຂອງທ່ານນໍາໃຊ້ລົດເປັນປົກກະຕິ?</t>
+  </si>
+  <si>
+    <t>ລວມທັງຕົວທ່ານເອງ, ຄົນໃນເຮືອນຂອງທ່ານມີຈັກຄົນທີ່ມີໃບຂັບຂີ່?</t>
+  </si>
+  <si>
+    <t>ຖ້າທ່ານບໍ່ສາມາດນໍາໃຊ້ພາຫະນະໃນເຮືອນຂອງທ່ານ (ຫຼືຖ້າບໍ່ມີທ່ານ), ທ່ານຈະເລືອກອັນໃດດັ່ງຕໍ່ໄປນີ້?</t>
+  </si>
+  <si>
+    <t>ທ່ານມີສະພາບທາງດ້ານຮ່າງກາຍ ທີ່ເຮັດໃຫ້ມັນມີຄວາມຫຍຸ້ງຍາກໃນການເດີນບໍ?</t>
+  </si>
+  <si>
+    <t>ທ່ານມີບັນຫາດ້ານຮ່າງກາຍດົນປານໃດ?</t>
+  </si>
+  <si>
+    <t>ຂໍ້ມູນທີ່ກ່ຽວຂ້ອງກັບວຽກຂອງທ່ານ</t>
+  </si>
+  <si>
+    <t>ທ່ານເຮັດວຽກເຕັມເວລາ ຫຼື ເຮັດວຽກລ່ວງເວລາ ບໍ?</t>
+  </si>
+  <si>
+    <t>ອັນໃດທີ່ບົ່ງບອກວ່າເປັນວຽກຫຼັກຂອງທ່ານ?</t>
+  </si>
+  <si>
+    <t>ຂໍໃຫ້ທ່ານໃຫ້ຂໍ້ມູນອັນທີ່ເປັນວຽກຫຼັກໆຂອງທ່ານ</t>
+  </si>
+  <si>
+    <t>ທ່ານມີຄວາມສາມາດໃນການກໍານົດຫຼືປ່ຽນເວລາເຂົ້າການດ້ວຍຕົວທ່ານເອງບໍ?</t>
+  </si>
+  <si>
+    <t>ທ່ານມີທາງເລືອກທີ່ຈະເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ໃດໜຶ່ງ ແທນທີ່ຈະເຂົ້າໄປເຮັດວຽກຢູ່ຫ້ອງການຂອງທ່ານ?</t>
+  </si>
+  <si>
+    <t>ປົກກະຕິມື້ໃດ ທີ່ທ່ານເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ອຶ່ນ ທີ່ບໍ່ແມ່ນຫ້ອງການຂອງທ່ານ</t>
+  </si>
+  <si>
+    <t>ປົກກະຕິຈັກວັນທ່ານເຮັດວຽກຢູ່ບ້ານ ຫລື ສະຖານທີ່ອຶ່ນ ທີ່ບໍ່ແມ່ນຫ້ອງການຂອງທ່ານ ຕໍ່ອາທິດ</t>
+  </si>
+  <si>
+    <t>ຂໍ້ມູນຂອງທ່ານ</t>
+  </si>
+  <si>
+    <t>ເພດຂອງທ່ານ?</t>
+  </si>
+  <si>
+    <t>ທ່ານຄິດວ່າທ່ານເອງເປັນ ຄົນຂ້າມເພດບໍ?</t>
+  </si>
+  <si>
+    <t>ຂໍ້ມູນໃດລຸ່ມນີ້ທີ່ກ່ຽວກັບທ່ານ?</t>
+  </si>
+  <si>
+    <t>ລະດັບການສຶກສາຂອງທ່ານ?</t>
+  </si>
+  <si>
+    <t>ທ່ານເປັນພະນັກງານບໍ?</t>
+  </si>
+  <si>
+    <t>ປະເພດເຮືອນຂອງທ່ານເປັນລັກສະນະແນວໃດ?</t>
+  </si>
+  <si>
+    <t>ທ່ານມີເຮືອນເປັນຂອງຕົນເອງບໍ ຫຼື ເຊົ່າເຮືອນເພີ່ນຢູ່?</t>
+  </si>
+  <si>
+    <t>ກະລຸນາເລືອກທັງໝົດ</t>
+  </si>
+  <si>
+    <t>ລວມທັງໂຮງຮຽນລັດ ແລະ ໂຮງຮຽນເອກະຊົນ ຫລື ຮຽນຢູ່ບ້ານ</t>
+  </si>
+  <si>
+    <t>ກະລຸນາລະບຸອັນໃດ ທີ່ເປັນລາຍຮັບຫຼັກໃນຄອບຂອງທ່ານ ສໍາລັບປີທີ່ຜ່ານມາ.</t>
+  </si>
+  <si>
+    <t>ເຫດຜົນທີ່ພວກເຮົາຖາມກ່ຽວກັບລາຍຮັບ ເນື່ອງຈາກເປັນພຽງການເກັບກໍາດ້ານສະຖິຕິ ໃນເວລາ ແລະ ວິທີການເດີນທາງ</t>
+  </si>
+  <si>
+    <t>ລວມທັງລົດຈັກ, ລົດຖີບທີ່ໃຊ້ມໍເຕີໄຟຟ້າ ແລະ ລົດບ້ານ</t>
+  </si>
+  <si>
+    <t>ພວກເຮົາໝາຍເຖີງ ເຮັດວຽກອຶ່ນນໍາ ເຊີ່ງີ່ມີຜູ້ທີ່ມາຈາ້ງທ່ານໃຫ້ເຮັດວຽກ (ທ່ານມີນາຍຈ້າງຫລາຍກ່ວາ 1)</t>
+  </si>
+  <si>
+    <t>ໃນເວລາທີ່ທ່ານເຮັດວຽກ ເຄີ່ງວັນ ຢູ່ເຮືອນ ຫລື ສະຖານທີ່ອຶ່ນ ແທນທີ່ບ່ອນເຮັດວຽກຂອງທ່ານ ແມ່ນຈະປັດໃຫ້ເປັນ 1 ວັນເລີຍ</t>
+  </si>
+  <si>
+    <t>16 ປີ ຫາ 20 ປີ</t>
+  </si>
+  <si>
+    <t>21 ປີ ຫາ 25 ປີ</t>
+  </si>
+  <si>
+    <t>26 ປີ ຫາ 30 ປີ</t>
+  </si>
+  <si>
+    <t>31 ປີ ຫາ 35 ປີ</t>
+  </si>
+  <si>
+    <t>36 ປີ ຫາ 40 ປີ</t>
+  </si>
+  <si>
+    <t>41 ປີ ຫາ 45 ປີ</t>
+  </si>
+  <si>
+    <t>46 ປີ ຫາ 50 ປີ</t>
+  </si>
+  <si>
+    <t>51 ປີ ຫາ 55 ປີ</t>
+  </si>
+  <si>
+    <t>56 ປີ ຫາ 60 ປີ</t>
+  </si>
+  <si>
+    <t>61 ປີ ຫາ 65 ປີ</t>
+  </si>
+  <si>
+    <t>ອາຍຸຕໍ່າກ່ວາ 16 ປີ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ອາຍຸຫລາຍກວ່າ 65 ປີ</t>
+  </si>
+  <si>
+    <t>ບໍ່ສະດວກໃຫ້ຂໍ້ມູນ</t>
+  </si>
+  <si>
+    <t>ເພດຊາຍ</t>
+  </si>
+  <si>
+    <t>ເພດຍິງ</t>
+  </si>
+  <si>
+    <t>ອຶ່ນໆ</t>
+  </si>
+  <si>
+    <t>ແມ່ນ</t>
+  </si>
+  <si>
+    <t>ບໍ່ແມ່ນ</t>
+  </si>
+  <si>
+    <t>ຄົນອາເມລິກາ ຜີວຂາວ</t>
+  </si>
+  <si>
+    <t>ຄົນອາເມລິກາ ຜີວດໍາ</t>
+  </si>
+  <si>
+    <t>ພາສາສະເປນ ຫລື ລາຕິນ</t>
+  </si>
+  <si>
+    <t>ອາຊີຕາເວັນອອກ</t>
+  </si>
+  <si>
+    <t>ອາຊີໄຕ້</t>
+  </si>
+  <si>
+    <t>ອິນເດຍ ອາເມລິກາ</t>
+  </si>
+  <si>
+    <t>ອາເມລິກາ ໃນໝູ່ເກາະຮາວາຍ</t>
+  </si>
+  <si>
+    <t>ຫລາຍເຊື້ອຊາດ</t>
+  </si>
+  <si>
+    <t>ບໍ່ແມ່ນ ນັກສຶກສາ</t>
+  </si>
+  <si>
+    <t>ແມ່ນ, ມັດທະຍົມສຶກສາ (ຕອນຕົ້ນ ແລະ ຕອນປາຍ)</t>
+  </si>
+  <si>
+    <t>ແມ່ນ, ການສຶກສາດ້ານວິຊາຊີບ</t>
+  </si>
+  <si>
+    <t>ແມ່ນ, ຮຽນເພີ້ມ ທີ່ວິທະຍາໄລ ຫລື ມະຫາວິທະຍາໄລ</t>
+  </si>
+  <si>
+    <t>ແມ່ນ, ຮຽນເຕັມເວລາ ທີ່ວິທະຍາໄລ ຫລື ມະຫາວິທະຍາໄລ</t>
+  </si>
+  <si>
+    <t>ຈົບການສຶກສາບໍ່ຮອດຂັ້ນມັດທະຍົມຕອນປາຍ</t>
+  </si>
+  <si>
+    <t>ຈົບການສຶກສາຊັ້ນສູງ</t>
+  </si>
+  <si>
+    <t>ຈົບການສຶກສາຂັ້ນມັດທະຍົມຕອນປາຍ</t>
+  </si>
+  <si>
+    <t>ຈົບການສຶກສາຂັ້ນ ປະລິນຍາຕີ</t>
+  </si>
+  <si>
+    <t>ຈົບການສຶກສາ ຂັ້ນປະລິນຍາໂທ ຫລື ສູງກ່ວາ</t>
+  </si>
+  <si>
+    <t>ຕອນນີ້ ຂ້ອຍຂາດວຽກຊົ່ວຄາວ</t>
+  </si>
+  <si>
+    <t>ຂ້ອຍບໍ່ສາມາດເຮັດວຽກໄດ້ ເນື່ອງຈາກສະພາບຮ່າງກາຍ, ກະສຽນແລ້ວ</t>
+  </si>
+  <si>
+    <t>ບໍ່ແມ່ນທັງໝົດ ຈາກຂ້າງເທີງ</t>
+  </si>
+  <si>
+    <t>ເປັນເຈົ້າຂອງເອງ</t>
+  </si>
+  <si>
+    <t>ເຊົ່າ</t>
+  </si>
+  <si>
+    <t>ບໍ່ແມ່ນທັງສອງ</t>
+  </si>
+  <si>
+    <t>ເຊົ່າອາຄານ ຫລື ເປັນອາພາດເມັນ</t>
+  </si>
+  <si>
+    <t>ສະເພາະຄອບຄົວເອງ</t>
+  </si>
+  <si>
+    <t>ມີຫລາຍຄອບຄົວອາໃສຢູ່ນໍາກັນ</t>
+  </si>
+  <si>
+    <t>ທີ່ລົບໄພ ຫລື ສະຖານທີ່ພັກຊົ່ວຄາວ</t>
+  </si>
+  <si>
+    <t>ຫລາຍກ່ວາ 7</t>
+  </si>
+  <si>
+    <t>ຫລາຍກ່ວາ 3</t>
+  </si>
+  <si>
+    <t>ຫລາຍກ່ວາ 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ການຂົນສົ່ງສາທາລະນະ (ລົດເມ, ລົດໄຟ) </t>
+  </si>
+  <si>
+    <t>ຂີ່ລົດໄປກັບໝູ່ ຫລື ຄົນໃນຄອບຄົວ ຫລື ໃນບ້ານດຽວກັນ</t>
+  </si>
+  <si>
+    <t>ເຊົ່າລົດ</t>
+  </si>
+  <si>
+    <t>ລົດຖີບ</t>
+  </si>
+  <si>
+    <t>ຍ່າງ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ແທັກຊີ </t>
+  </si>
+  <si>
+    <t>ບໍ່ມີ</t>
+  </si>
+  <si>
+    <t>6 ເດືອນ ຫລື ໜ້ອຍກ່ວາ</t>
+  </si>
+  <si>
+    <t>ຫລາຍກ່ວາ 6 ເດືອນ</t>
+  </si>
+  <si>
+    <t>ຕະຫລອດຊີວິດ</t>
+  </si>
+  <si>
+    <t>ເຕັມເວລາ</t>
+  </si>
+  <si>
+    <t>ລ່ວງເວລາ</t>
+  </si>
+  <si>
+    <t>ການຂາຍ ຫລື ວຽກບໍລິການ</t>
+  </si>
+  <si>
+    <t>ວຽກບໍລິຫານ</t>
+  </si>
+  <si>
+    <t>ວຽກໂຮງງານ, ການກໍໍ່ສ້າງ ຫລື ກະສິກໍາ</t>
+  </si>
+  <si>
+    <t>ວິຊາຊີບສະເພາະ, ການຈັດການ, ຫລື ເປັນຊ່າງຊໍານານງານສະເພາະດ້ານ</t>
+  </si>
+  <si>
+    <t>ວັນຈັນ</t>
+  </si>
+  <si>
+    <t>ວັນອັງຄານ</t>
+  </si>
+  <si>
+    <t>ວັນພຸດ</t>
+  </si>
+  <si>
+    <t>ວັນພະຫັດ</t>
+  </si>
+  <si>
+    <t>ວັນສຸກ</t>
+  </si>
+  <si>
+    <t>ວັນອາທິດ</t>
+  </si>
+  <si>
+    <t>ວັນເສົາ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1359,13 +1773,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Phetsarath OT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Phet"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Saysettha OT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1380,21 +1829,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1432,7 +1897,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1466,6 +1931,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1500,9 +1966,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1675,14 +2142,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="4" max="4" width="105.44140625" customWidth="1"/>
+    <col min="5" max="5" width="65.5546875" customWidth="1"/>
+    <col min="6" max="6" width="50.21875" customWidth="1"/>
+    <col min="7" max="7" width="73.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="147.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,45 +2171,57 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12" ht="22.8">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="D2" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="22.8">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="D3" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="22.8">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1740,14 +2231,17 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12" ht="22.8">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1757,14 +2251,17 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12" ht="22.8">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1774,14 +2271,17 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12" ht="22.8">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1791,17 +2291,20 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12" ht="22.8">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1811,20 +2314,26 @@
       <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12" ht="22.8">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1834,14 +2343,17 @@
       <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:12" ht="22.8">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1851,20 +2363,26 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="H10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:12" ht="22.8">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1874,14 +2392,17 @@
       <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:12" ht="22.8">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1891,14 +2412,17 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E12" t="s">
         <v>54</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:12" ht="22.8">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1908,22 +2432,26 @@
       <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:12" ht="22.8">
       <c r="A14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="22.8">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1933,14 +2461,17 @@
       <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E15" t="s">
         <v>63</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:12" ht="22.8">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1950,14 +2481,17 @@
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:11" ht="22.8">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1967,14 +2501,17 @@
       <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="E17" t="s">
         <v>71</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:11" ht="22.8">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1984,20 +2521,26 @@
       <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E18" t="s">
         <v>75</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>76</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="H18" t="s">
         <v>77</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11" ht="22.8">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -2007,14 +2550,17 @@
       <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E19" t="s">
         <v>81</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11" ht="22.8">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2024,14 +2570,17 @@
       <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E20" t="s">
         <v>85</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11" ht="22.8">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2041,14 +2590,17 @@
       <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" t="s">
         <v>88</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:11" ht="22.8">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -2058,14 +2610,17 @@
       <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="E22" t="s">
         <v>92</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11" ht="22.8">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2075,20 +2630,26 @@
       <c r="C23" t="s">
         <v>95</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="E23" t="s">
         <v>96</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>97</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="H23" t="s">
         <v>98</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:11" ht="22.8">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2098,14 +2659,17 @@
       <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E24" t="s">
         <v>102</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:11" ht="22.8">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -2115,14 +2679,17 @@
       <c r="C25" t="s">
         <v>105</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="E25" t="s">
         <v>106</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:11" ht="22.8">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -2132,22 +2699,26 @@
       <c r="C26" t="s">
         <v>109</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="E26" t="s">
         <v>110</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>21</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:11" ht="22.8">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="22.8">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2157,17 +2728,20 @@
       <c r="C28" t="s">
         <v>113</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E28" t="s">
         <v>114</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>16</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:11" ht="22.8">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -2177,20 +2751,26 @@
       <c r="C29" t="s">
         <v>118</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E29" t="s">
         <v>119</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>120</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="H29" t="s">
         <v>121</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11" ht="22.8">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -2200,20 +2780,23 @@
       <c r="C30" t="s">
         <v>124</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="E30" t="s">
         <v>125</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>126</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>127</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:11" ht="22.8">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -2223,14 +2806,17 @@
       <c r="C31" t="s">
         <v>130</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E31" t="s">
         <v>131</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:11" ht="22.8">
       <c r="A32" t="s">
         <v>132</v>
       </c>
@@ -2240,23 +2826,26 @@
       <c r="C32" t="s">
         <v>134</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E32" t="s">
         <v>135</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>136</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>137</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>16</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:12" ht="22.8">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -2266,14 +2855,17 @@
       <c r="C33" t="s">
         <v>141</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E33" t="s">
         <v>142</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:12" ht="22.8">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -2283,14 +2875,17 @@
       <c r="C34" t="s">
         <v>145</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="E34" t="s">
         <v>146</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:12" ht="22.8">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -2300,23 +2895,29 @@
       <c r="C35" t="s">
         <v>149</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="E35" t="s">
         <v>150</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>151</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="H35" t="s">
         <v>152</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>21</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:12" ht="22.8">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -2326,52 +2927,79 @@
       <c r="C36" t="s">
         <v>156</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E36" t="s">
         <v>157</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>35</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H36" t="s">
         <v>36</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>21</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:12" ht="22.8">
       <c r="A37" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" ht="22.8">
       <c r="A38" t="s">
         <v>159</v>
       </c>
       <c r="B38" t="s">
         <v>160</v>
       </c>
-      <c r="J38" t="s">
+      <c r="D38" s="3"/>
+      <c r="L38" t="s">
         <v>161</v>
       </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="D40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="12" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <customProperties>
+    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" customWidth="1"/>
+    <col min="4" max="4" width="40.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="68.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>162</v>
       </c>
@@ -2381,14 +3009,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>164</v>
       </c>
@@ -2398,11 +3029,14 @@
       <c r="C2" t="s">
         <v>166</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -2412,11 +3046,14 @@
       <c r="C3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2426,11 +3063,14 @@
       <c r="C4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -2440,11 +3080,14 @@
       <c r="C5" t="s">
         <v>175</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -2454,11 +3097,14 @@
       <c r="C6" t="s">
         <v>178</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -2468,11 +3114,14 @@
       <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -2482,11 +3131,14 @@
       <c r="C8" t="s">
         <v>184</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -2496,11 +3148,14 @@
       <c r="C9" t="s">
         <v>187</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E9" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -2510,11 +3165,14 @@
       <c r="C10" t="s">
         <v>190</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -2524,11 +3182,14 @@
       <c r="C11" t="s">
         <v>193</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -2538,11 +3199,14 @@
       <c r="C12" t="s">
         <v>196</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="E12" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -2552,11 +3216,14 @@
       <c r="C13" t="s">
         <v>199</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -2566,11 +3233,14 @@
       <c r="C14" t="s">
         <v>202</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E14" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -2580,11 +3250,14 @@
       <c r="C15" t="s">
         <v>206</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="E15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -2594,11 +3267,14 @@
       <c r="C16" t="s">
         <v>209</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E16" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -2608,11 +3284,14 @@
       <c r="C17" t="s">
         <v>212</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>204</v>
       </c>
@@ -2622,11 +3301,14 @@
       <c r="C18" t="s">
         <v>215</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E18" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -2636,11 +3318,14 @@
       <c r="C19" t="s">
         <v>202</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E19" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -2650,11 +3335,14 @@
       <c r="C20" t="s">
         <v>219</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>217</v>
       </c>
@@ -2664,11 +3352,14 @@
       <c r="C21" t="s">
         <v>221</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>217</v>
       </c>
@@ -2678,53 +3369,65 @@
       <c r="C22" t="s">
         <v>202</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E22" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>222</v>
       </c>
       <c r="B23" t="s">
         <v>223</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="E23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>222</v>
       </c>
       <c r="B24" t="s">
         <v>226</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E24" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>222</v>
       </c>
       <c r="B25" t="s">
         <v>229</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E25" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>222</v>
       </c>
@@ -2734,11 +3437,14 @@
       <c r="C26" t="s">
         <v>233</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E26" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>222</v>
       </c>
@@ -2748,11 +3454,14 @@
       <c r="C27" t="s">
         <v>236</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>222</v>
       </c>
@@ -2762,11 +3471,14 @@
       <c r="C28" t="s">
         <v>239</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="E28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>222</v>
       </c>
@@ -2776,11 +3488,14 @@
       <c r="C29" t="s">
         <v>242</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E29" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>222</v>
       </c>
@@ -2790,11 +3505,14 @@
       <c r="C30" t="s">
         <v>245</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E30" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>222</v>
       </c>
@@ -2804,11 +3522,14 @@
       <c r="C31" t="s">
         <v>215</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E31" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>222</v>
       </c>
@@ -2818,11 +3539,14 @@
       <c r="C32" t="s">
         <v>202</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E32" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -2832,11 +3556,14 @@
       <c r="C33" t="s">
         <v>219</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E33" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -2846,11 +3573,14 @@
       <c r="C34" t="s">
         <v>221</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E34" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -2860,11 +3590,14 @@
       <c r="C35" t="s">
         <v>202</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E35" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>249</v>
       </c>
@@ -2874,11 +3607,14 @@
       <c r="C36" t="s">
         <v>251</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E36" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>249</v>
       </c>
@@ -2888,11 +3624,14 @@
       <c r="C37" t="s">
         <v>254</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E37" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>249</v>
       </c>
@@ -2902,11 +3641,14 @@
       <c r="C38" t="s">
         <v>257</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E38" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>249</v>
       </c>
@@ -2916,11 +3658,14 @@
       <c r="C39" t="s">
         <v>260</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E39" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>249</v>
       </c>
@@ -2930,11 +3675,14 @@
       <c r="C40" t="s">
         <v>263</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E40" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>249</v>
       </c>
@@ -2944,11 +3692,14 @@
       <c r="C41" t="s">
         <v>202</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E41" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>265</v>
       </c>
@@ -2958,11 +3709,14 @@
       <c r="C42" t="s">
         <v>267</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E42" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>265</v>
       </c>
@@ -2972,11 +3726,14 @@
       <c r="C43" t="s">
         <v>270</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="E43" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>265</v>
       </c>
@@ -2986,11 +3743,14 @@
       <c r="C44" t="s">
         <v>273</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E44" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>265</v>
       </c>
@@ -3000,11 +3760,14 @@
       <c r="C45" t="s">
         <v>276</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E45" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>265</v>
       </c>
@@ -3014,11 +3777,14 @@
       <c r="C46" t="s">
         <v>279</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E46" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>265</v>
       </c>
@@ -3028,11 +3794,14 @@
       <c r="C47" t="s">
         <v>202</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E47" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>281</v>
       </c>
@@ -3042,11 +3811,14 @@
       <c r="C48" t="s">
         <v>219</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E48" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>281</v>
       </c>
@@ -3056,11 +3828,14 @@
       <c r="C49" t="s">
         <v>221</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E49" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>281</v>
       </c>
@@ -3070,11 +3845,14 @@
       <c r="C50" t="s">
         <v>202</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E50" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>283</v>
       </c>
@@ -3084,11 +3862,14 @@
       <c r="C51" t="s">
         <v>285</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E51" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>283</v>
       </c>
@@ -3098,14 +3879,17 @@
       <c r="C52" t="s">
         <v>288</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E52" t="s">
         <v>289</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -3115,14 +3899,17 @@
       <c r="C53" t="s">
         <v>291</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="E53" t="s">
         <v>292</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>283</v>
       </c>
@@ -3132,14 +3919,17 @@
       <c r="C54" t="s">
         <v>202</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E54" t="s">
         <v>203</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>293</v>
       </c>
@@ -3149,11 +3939,14 @@
       <c r="C55" t="s">
         <v>295</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E55" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>293</v>
       </c>
@@ -3163,14 +3956,17 @@
       <c r="C56" t="s">
         <v>298</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E56" t="s">
         <v>299</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>293</v>
       </c>
@@ -3180,14 +3976,17 @@
       <c r="C57" t="s">
         <v>301</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E57" t="s">
         <v>302</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>293</v>
       </c>
@@ -3197,14 +3996,17 @@
       <c r="C58" t="s">
         <v>202</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E58" t="s">
         <v>203</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>303</v>
       </c>
@@ -3214,11 +4016,14 @@
       <c r="C59" t="s">
         <v>305</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="E59" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>303</v>
       </c>
@@ -3228,14 +4033,17 @@
       <c r="C60" t="s">
         <v>308</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E60" t="s">
         <v>309</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>303</v>
       </c>
@@ -3245,14 +4053,17 @@
       <c r="C61" t="s">
         <v>311</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E61" t="s">
         <v>312</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -3262,14 +4073,17 @@
       <c r="C62" t="s">
         <v>314</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="E62" t="s">
         <v>315</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>303</v>
       </c>
@@ -3279,98 +4093,101 @@
       <c r="C63" t="s">
         <v>202</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E63" t="s">
         <v>203</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>316</v>
       </c>
       <c r="B64" t="s">
         <v>317</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>316</v>
       </c>
       <c r="B65" t="s">
         <v>320</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>316</v>
       </c>
       <c r="B66" t="s">
         <v>323</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>316</v>
       </c>
       <c r="B67" t="s">
         <v>326</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>316</v>
       </c>
       <c r="B68" t="s">
         <v>329</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>316</v>
       </c>
       <c r="B69" t="s">
         <v>332</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>316</v>
       </c>
@@ -3380,11 +4197,14 @@
       <c r="C70" t="s">
         <v>202</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E70" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>335</v>
       </c>
@@ -3394,11 +4214,14 @@
       <c r="C71" t="s">
         <v>336</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="5">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>335</v>
       </c>
@@ -3408,11 +4231,14 @@
       <c r="C72" t="s">
         <v>337</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="5">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>335</v>
       </c>
@@ -3422,11 +4248,14 @@
       <c r="C73" t="s">
         <v>338</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="5">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>335</v>
       </c>
@@ -3436,11 +4265,14 @@
       <c r="C74" t="s">
         <v>339</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="5">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>335</v>
       </c>
@@ -3450,11 +4282,14 @@
       <c r="C75" t="s">
         <v>340</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="5">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>335</v>
       </c>
@@ -3464,11 +4299,14 @@
       <c r="C76" t="s">
         <v>341</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="5">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>335</v>
       </c>
@@ -3478,11 +4316,14 @@
       <c r="C77" t="s">
         <v>342</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="5">
+        <v>7</v>
+      </c>
+      <c r="E77" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>335</v>
       </c>
@@ -3492,11 +4333,14 @@
       <c r="C78" t="s">
         <v>344</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="E78" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>335</v>
       </c>
@@ -3506,11 +4350,14 @@
       <c r="C79" t="s">
         <v>202</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E79" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>346</v>
       </c>
@@ -3520,11 +4367,14 @@
       <c r="C80" t="s">
         <v>347</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="E80" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>346</v>
       </c>
@@ -3534,14 +4384,17 @@
       <c r="C81" t="s">
         <v>336</v>
       </c>
-      <c r="D81" t="s">
-        <v>336</v>
+      <c r="D81" s="5">
+        <v>1</v>
       </c>
       <c r="E81" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>346</v>
       </c>
@@ -3551,14 +4404,17 @@
       <c r="C82" t="s">
         <v>337</v>
       </c>
-      <c r="D82" t="s">
-        <v>337</v>
+      <c r="D82" s="5">
+        <v>2</v>
       </c>
       <c r="E82" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -3568,14 +4424,17 @@
       <c r="C83" t="s">
         <v>338</v>
       </c>
-      <c r="D83" t="s">
-        <v>338</v>
+      <c r="D83" s="5">
+        <v>3</v>
       </c>
       <c r="E83" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>346</v>
       </c>
@@ -3585,14 +4444,17 @@
       <c r="C84" t="s">
         <v>339</v>
       </c>
-      <c r="D84" t="s">
-        <v>339</v>
+      <c r="D84" s="5">
+        <v>4</v>
       </c>
       <c r="E84" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>346</v>
       </c>
@@ -3602,14 +4464,17 @@
       <c r="C85" t="s">
         <v>349</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E85" t="s">
         <v>350</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>346</v>
       </c>
@@ -3619,14 +4484,17 @@
       <c r="C86" t="s">
         <v>202</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="E86" t="s">
         <v>203</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>351</v>
       </c>
@@ -3636,11 +4504,14 @@
       <c r="C87" t="s">
         <v>347</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="E87" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>351</v>
       </c>
@@ -3650,11 +4521,14 @@
       <c r="C88" t="s">
         <v>336</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="5">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>351</v>
       </c>
@@ -3664,11 +4538,14 @@
       <c r="C89" t="s">
         <v>337</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="5">
+        <v>2</v>
+      </c>
+      <c r="E89" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>351</v>
       </c>
@@ -3678,11 +4555,14 @@
       <c r="C90" t="s">
         <v>338</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="5">
+        <v>3</v>
+      </c>
+      <c r="E90" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>351</v>
       </c>
@@ -3692,11 +4572,14 @@
       <c r="C91" t="s">
         <v>339</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="5">
+        <v>4</v>
+      </c>
+      <c r="E91" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>351</v>
       </c>
@@ -3706,11 +4589,14 @@
       <c r="C92" t="s">
         <v>349</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E92" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>351</v>
       </c>
@@ -3720,11 +4606,14 @@
       <c r="C93" t="s">
         <v>202</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E93" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>352</v>
       </c>
@@ -3734,11 +4623,14 @@
       <c r="C94" t="s">
         <v>347</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="E94" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>352</v>
       </c>
@@ -3748,11 +4640,14 @@
       <c r="C95" t="s">
         <v>336</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="5">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>352</v>
       </c>
@@ -3762,11 +4657,14 @@
       <c r="C96" t="s">
         <v>337</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="5">
+        <v>2</v>
+      </c>
+      <c r="E96" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>352</v>
       </c>
@@ -3776,11 +4674,14 @@
       <c r="C97" t="s">
         <v>338</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="5">
+        <v>3</v>
+      </c>
+      <c r="E97" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>352</v>
       </c>
@@ -3790,11 +4691,14 @@
       <c r="C98" t="s">
         <v>354</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="E98" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>352</v>
       </c>
@@ -3804,11 +4708,14 @@
       <c r="C99" t="s">
         <v>202</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E99" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>356</v>
       </c>
@@ -3818,11 +4725,14 @@
       <c r="C100" t="s">
         <v>358</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E100" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>356</v>
       </c>
@@ -3832,11 +4742,14 @@
       <c r="C101" t="s">
         <v>361</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E101" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>356</v>
       </c>
@@ -3846,11 +4759,14 @@
       <c r="C102" t="s">
         <v>364</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E102" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>356</v>
       </c>
@@ -3860,11 +4776,14 @@
       <c r="C103" t="s">
         <v>367</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E103" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>356</v>
       </c>
@@ -3874,11 +4793,14 @@
       <c r="C104" t="s">
         <v>370</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E104" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>356</v>
       </c>
@@ -3888,11 +4810,14 @@
       <c r="C105" t="s">
         <v>373</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="E105" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>356</v>
       </c>
@@ -3902,11 +4827,14 @@
       <c r="C106" t="s">
         <v>376</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E106" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>356</v>
       </c>
@@ -3916,11 +4844,14 @@
       <c r="C107" t="s">
         <v>202</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E107" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>377</v>
       </c>
@@ -3930,11 +4861,14 @@
       <c r="C108" t="s">
         <v>219</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E108" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>377</v>
       </c>
@@ -3944,11 +4878,14 @@
       <c r="C109" t="s">
         <v>221</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E109" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>377</v>
       </c>
@@ -3958,11 +4895,14 @@
       <c r="C110" t="s">
         <v>202</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E110" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>378</v>
       </c>
@@ -3972,11 +4912,14 @@
       <c r="C111" t="s">
         <v>380</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E111" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>378</v>
       </c>
@@ -3986,11 +4929,14 @@
       <c r="C112" t="s">
         <v>383</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E112" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -4000,11 +4946,14 @@
       <c r="C113" t="s">
         <v>386</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="E113" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>378</v>
       </c>
@@ -4014,11 +4963,14 @@
       <c r="C114" t="s">
         <v>202</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E114" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>389</v>
       </c>
@@ -4028,11 +4980,14 @@
       <c r="C115" t="s">
         <v>219</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E115" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>389</v>
       </c>
@@ -4042,11 +4997,14 @@
       <c r="C116" t="s">
         <v>221</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E116" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>389</v>
       </c>
@@ -4056,11 +5014,14 @@
       <c r="C117" t="s">
         <v>202</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E117" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>390</v>
       </c>
@@ -4070,11 +5031,14 @@
       <c r="C118" t="s">
         <v>392</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E118" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>390</v>
       </c>
@@ -4084,11 +5048,14 @@
       <c r="C119" t="s">
         <v>395</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="E119" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>390</v>
       </c>
@@ -4098,11 +5065,14 @@
       <c r="C120" t="s">
         <v>202</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E120" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>397</v>
       </c>
@@ -4112,11 +5082,14 @@
       <c r="C121" t="s">
         <v>399</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E121" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>397</v>
       </c>
@@ -4126,11 +5099,14 @@
       <c r="C122" t="s">
         <v>402</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E122" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>397</v>
       </c>
@@ -4140,11 +5116,14 @@
       <c r="C123" t="s">
         <v>405</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E123" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>397</v>
       </c>
@@ -4154,11 +5133,14 @@
       <c r="C124" t="s">
         <v>408</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E124" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>397</v>
       </c>
@@ -4168,11 +5150,14 @@
       <c r="C125" t="s">
         <v>215</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E125" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>397</v>
       </c>
@@ -4182,11 +5167,14 @@
       <c r="C126" t="s">
         <v>202</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E126" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>410</v>
       </c>
@@ -4196,11 +5184,14 @@
       <c r="C127" t="s">
         <v>219</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E127" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -4210,11 +5201,14 @@
       <c r="C128" t="s">
         <v>221</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E128" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>410</v>
       </c>
@@ -4224,11 +5218,14 @@
       <c r="C129" t="s">
         <v>202</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E129" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>411</v>
       </c>
@@ -4238,11 +5235,14 @@
       <c r="C130" t="s">
         <v>219</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E130" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>411</v>
       </c>
@@ -4252,11 +5252,14 @@
       <c r="C131" t="s">
         <v>221</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E131" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>411</v>
       </c>
@@ -4266,11 +5269,14 @@
       <c r="C132" t="s">
         <v>202</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E132" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>412</v>
       </c>
@@ -4280,11 +5286,14 @@
       <c r="C133" t="s">
         <v>347</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="6" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>412</v>
       </c>
@@ -4294,11 +5303,14 @@
       <c r="C134" t="s">
         <v>336</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="5">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>412</v>
       </c>
@@ -4308,11 +5320,14 @@
       <c r="C135" t="s">
         <v>337</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="5">
+        <v>2</v>
+      </c>
+      <c r="E135" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>412</v>
       </c>
@@ -4322,11 +5337,14 @@
       <c r="C136" t="s">
         <v>338</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="5">
+        <v>3</v>
+      </c>
+      <c r="E136" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>412</v>
       </c>
@@ -4336,11 +5354,14 @@
       <c r="C137" t="s">
         <v>339</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="5">
+        <v>4</v>
+      </c>
+      <c r="E137" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>412</v>
       </c>
@@ -4350,11 +5371,14 @@
       <c r="C138" t="s">
         <v>340</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="5">
+        <v>5</v>
+      </c>
+      <c r="E138" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>412</v>
       </c>
@@ -4364,11 +5388,14 @@
       <c r="C139" t="s">
         <v>341</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="5">
+        <v>6</v>
+      </c>
+      <c r="E139" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>412</v>
       </c>
@@ -4378,11 +5405,14 @@
       <c r="C140" t="s">
         <v>342</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="5">
+        <v>7</v>
+      </c>
+      <c r="E140" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>412</v>
       </c>
@@ -4392,11 +5422,14 @@
       <c r="C141" t="s">
         <v>202</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E141" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>413</v>
       </c>
@@ -4406,11 +5439,14 @@
       <c r="C142" t="s">
         <v>415</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E142" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>413</v>
       </c>
@@ -4420,11 +5456,14 @@
       <c r="C143" t="s">
         <v>418</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E143" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>413</v>
       </c>
@@ -4434,11 +5473,14 @@
       <c r="C144" t="s">
         <v>421</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E144" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>413</v>
       </c>
@@ -4448,11 +5490,14 @@
       <c r="C145" t="s">
         <v>424</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E145" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>413</v>
       </c>
@@ -4462,11 +5507,14 @@
       <c r="C146" t="s">
         <v>427</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E146" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>413</v>
       </c>
@@ -4476,11 +5524,14 @@
       <c r="C147" t="s">
         <v>430</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E147" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>413</v>
       </c>
@@ -4490,11 +5541,14 @@
       <c r="C148" t="s">
         <v>433</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E148" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>413</v>
       </c>
@@ -4504,22 +5558,29 @@
       <c r="C149" t="s">
         <v>202</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E149" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId1"/>
+  </customProperties>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -4551,5 +5612,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="QAA_DRILLPATH_NODE_ID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
unify Lao hints with Qs and As
I found another mistake in the column names, the hint column was different than the rest of the Lao columns, so it was reading as 2 Lao options (one for questions and answers and one for hints) this should fix but needs a json conversion!
</commit_message>
<xml_diff>
--- a/survey-resources/data-xls/demo-survey-v2.xlsx
+++ b/survey-resources/data-xls/demo-survey-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awheelis/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFAA68E9-B742-4446-8383-1B302A7DCEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1677AFD6-E010-AB48-91B0-5ADF5F39E206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32540" yWindow="2020" windowWidth="28800" windowHeight="15780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32540" yWindow="2020" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1419,9 +1419,6 @@
     <t>English (en)</t>
   </si>
   <si>
-    <t xml:space="preserve">hint::ລາວ (lao) </t>
-  </si>
-  <si>
     <t>ເລີ້ມອອກເດີນທາງ</t>
   </si>
   <si>
@@ -1756,6 +1753,9 @@
   </si>
   <si>
     <t xml:space="preserve">label::ລາວ (lo) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint::ລາວ (lo) </t>
   </si>
 </sst>
 </file>
@@ -2142,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2169,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2178,7 +2178,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>443</v>
+        <v>555</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -2204,7 +2204,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2215,7 +2215,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2229,7 +2229,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -2249,7 +2249,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -2269,7 +2269,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -2289,7 +2289,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -2312,7 +2312,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
@@ -2321,7 +2321,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -2341,7 +2341,7 @@
         <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -2361,7 +2361,7 @@
         <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E10" t="s">
         <v>44</v>
@@ -2370,7 +2370,7 @@
         <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H10" t="s">
         <v>46</v>
@@ -2390,7 +2390,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E11" t="s">
         <v>50</v>
@@ -2410,7 +2410,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -2430,7 +2430,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
@@ -2459,7 +2459,7 @@
         <v>62</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E15" t="s">
         <v>63</v>
@@ -2479,7 +2479,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E16" t="s">
         <v>67</v>
@@ -2499,7 +2499,7 @@
         <v>70</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E17" t="s">
         <v>71</v>
@@ -2519,7 +2519,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E18" t="s">
         <v>75</v>
@@ -2528,7 +2528,7 @@
         <v>76</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H18" t="s">
         <v>77</v>
@@ -2548,7 +2548,7 @@
         <v>80</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E19" t="s">
         <v>81</v>
@@ -2568,7 +2568,7 @@
         <v>84</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E20" t="s">
         <v>85</v>
@@ -2588,7 +2588,7 @@
         <v>87</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E21" t="s">
         <v>88</v>
@@ -2608,7 +2608,7 @@
         <v>91</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E22" t="s">
         <v>92</v>
@@ -2628,7 +2628,7 @@
         <v>95</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E23" t="s">
         <v>96</v>
@@ -2637,7 +2637,7 @@
         <v>97</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H23" t="s">
         <v>98</v>
@@ -2657,7 +2657,7 @@
         <v>101</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E24" t="s">
         <v>102</v>
@@ -2677,7 +2677,7 @@
         <v>105</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E25" t="s">
         <v>106</v>
@@ -2697,7 +2697,7 @@
         <v>109</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E26" t="s">
         <v>110</v>
@@ -2726,7 +2726,7 @@
         <v>113</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E28" t="s">
         <v>114</v>
@@ -2749,7 +2749,7 @@
         <v>118</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E29" t="s">
         <v>119</v>
@@ -2758,7 +2758,7 @@
         <v>120</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H29" t="s">
         <v>121</v>
@@ -2778,7 +2778,7 @@
         <v>124</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E30" t="s">
         <v>125</v>
@@ -2804,7 +2804,7 @@
         <v>130</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E31" t="s">
         <v>131</v>
@@ -2824,7 +2824,7 @@
         <v>134</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E32" t="s">
         <v>135</v>
@@ -2853,7 +2853,7 @@
         <v>141</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E33" t="s">
         <v>142</v>
@@ -2873,7 +2873,7 @@
         <v>145</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E34" t="s">
         <v>146</v>
@@ -2893,7 +2893,7 @@
         <v>149</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E35" t="s">
         <v>150</v>
@@ -2902,7 +2902,7 @@
         <v>151</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H35" t="s">
         <v>152</v>
@@ -2925,7 +2925,7 @@
         <v>156</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E36" t="s">
         <v>157</v>
@@ -2934,7 +2934,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H36" t="s">
         <v>36</v>
@@ -2983,7 +2983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3007,7 +3007,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3027,7 +3027,7 @@
         <v>166</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E2" t="s">
         <v>167</v>
@@ -3044,7 +3044,7 @@
         <v>169</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E3" t="s">
         <v>170</v>
@@ -3061,7 +3061,7 @@
         <v>172</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E4" t="s">
         <v>173</v>
@@ -3078,7 +3078,7 @@
         <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E5" t="s">
         <v>176</v>
@@ -3095,7 +3095,7 @@
         <v>178</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E6" t="s">
         <v>179</v>
@@ -3112,7 +3112,7 @@
         <v>181</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E7" t="s">
         <v>182</v>
@@ -3129,7 +3129,7 @@
         <v>184</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E8" t="s">
         <v>185</v>
@@ -3146,7 +3146,7 @@
         <v>187</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E9" t="s">
         <v>188</v>
@@ -3163,7 +3163,7 @@
         <v>190</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E10" t="s">
         <v>191</v>
@@ -3180,7 +3180,7 @@
         <v>193</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E11" t="s">
         <v>194</v>
@@ -3197,7 +3197,7 @@
         <v>196</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E12" t="s">
         <v>197</v>
@@ -3214,7 +3214,7 @@
         <v>199</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E13" t="s">
         <v>200</v>
@@ -3231,7 +3231,7 @@
         <v>202</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E14" t="s">
         <v>203</v>
@@ -3248,7 +3248,7 @@
         <v>206</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E15" t="s">
         <v>207</v>
@@ -3265,7 +3265,7 @@
         <v>209</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E16" t="s">
         <v>210</v>
@@ -3282,7 +3282,7 @@
         <v>212</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E17" t="s">
         <v>213</v>
@@ -3299,7 +3299,7 @@
         <v>215</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E18" t="s">
         <v>216</v>
@@ -3316,7 +3316,7 @@
         <v>202</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E19" t="s">
         <v>203</v>
@@ -3333,7 +3333,7 @@
         <v>219</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E20" t="s">
         <v>210</v>
@@ -3350,7 +3350,7 @@
         <v>221</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E21" t="s">
         <v>207</v>
@@ -3367,7 +3367,7 @@
         <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E22" t="s">
         <v>203</v>
@@ -3384,7 +3384,7 @@
         <v>224</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E23" t="s">
         <v>225</v>
@@ -3401,7 +3401,7 @@
         <v>227</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E24" t="s">
         <v>228</v>
@@ -3418,7 +3418,7 @@
         <v>230</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E25" t="s">
         <v>231</v>
@@ -3435,7 +3435,7 @@
         <v>233</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E26" t="s">
         <v>234</v>
@@ -3452,7 +3452,7 @@
         <v>236</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E27" t="s">
         <v>237</v>
@@ -3469,7 +3469,7 @@
         <v>239</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E28" t="s">
         <v>240</v>
@@ -3486,7 +3486,7 @@
         <v>242</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E29" t="s">
         <v>243</v>
@@ -3503,7 +3503,7 @@
         <v>245</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E30" t="s">
         <v>246</v>
@@ -3520,7 +3520,7 @@
         <v>215</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E31" t="s">
         <v>216</v>
@@ -3537,7 +3537,7 @@
         <v>202</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E32" t="s">
         <v>203</v>
@@ -3554,7 +3554,7 @@
         <v>219</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E33" t="s">
         <v>248</v>
@@ -3571,7 +3571,7 @@
         <v>221</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E34" t="s">
         <v>221</v>
@@ -3588,7 +3588,7 @@
         <v>202</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E35" t="s">
         <v>203</v>
@@ -3605,7 +3605,7 @@
         <v>251</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E36" t="s">
         <v>252</v>
@@ -3622,7 +3622,7 @@
         <v>254</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E37" t="s">
         <v>255</v>
@@ -3639,7 +3639,7 @@
         <v>257</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E38" t="s">
         <v>258</v>
@@ -3656,7 +3656,7 @@
         <v>260</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E39" t="s">
         <v>261</v>
@@ -3673,7 +3673,7 @@
         <v>263</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E40" t="s">
         <v>264</v>
@@ -3690,7 +3690,7 @@
         <v>202</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E41" t="s">
         <v>203</v>
@@ -3707,7 +3707,7 @@
         <v>267</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E42" t="s">
         <v>268</v>
@@ -3724,7 +3724,7 @@
         <v>270</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E43" t="s">
         <v>271</v>
@@ -3741,7 +3741,7 @@
         <v>273</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E44" t="s">
         <v>274</v>
@@ -3758,7 +3758,7 @@
         <v>276</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E45" t="s">
         <v>277</v>
@@ -3775,7 +3775,7 @@
         <v>279</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E46" t="s">
         <v>280</v>
@@ -3792,7 +3792,7 @@
         <v>202</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E47" t="s">
         <v>203</v>
@@ -3809,7 +3809,7 @@
         <v>219</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E48" t="s">
         <v>282</v>
@@ -3826,7 +3826,7 @@
         <v>221</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E49" t="s">
         <v>221</v>
@@ -3843,7 +3843,7 @@
         <v>202</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E50" t="s">
         <v>203</v>
@@ -3860,7 +3860,7 @@
         <v>285</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E51" t="s">
         <v>286</v>
@@ -3877,7 +3877,7 @@
         <v>288</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E52" t="s">
         <v>289</v>
@@ -3897,7 +3897,7 @@
         <v>291</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E53" t="s">
         <v>292</v>
@@ -3917,7 +3917,7 @@
         <v>202</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E54" t="s">
         <v>203</v>
@@ -3937,7 +3937,7 @@
         <v>295</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E55" t="s">
         <v>296</v>
@@ -3954,7 +3954,7 @@
         <v>298</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E56" t="s">
         <v>299</v>
@@ -3974,7 +3974,7 @@
         <v>301</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E57" t="s">
         <v>302</v>
@@ -3994,7 +3994,7 @@
         <v>202</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E58" t="s">
         <v>203</v>
@@ -4014,7 +4014,7 @@
         <v>305</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E59" t="s">
         <v>306</v>
@@ -4031,7 +4031,7 @@
         <v>308</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E60" t="s">
         <v>309</v>
@@ -4051,7 +4051,7 @@
         <v>311</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E61" t="s">
         <v>312</v>
@@ -4071,7 +4071,7 @@
         <v>314</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E62" t="s">
         <v>315</v>
@@ -4091,7 +4091,7 @@
         <v>202</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E63" t="s">
         <v>203</v>
@@ -4195,7 +4195,7 @@
         <v>202</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E70" t="s">
         <v>203</v>
@@ -4331,7 +4331,7 @@
         <v>344</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E78" t="s">
         <v>345</v>
@@ -4348,7 +4348,7 @@
         <v>202</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E79" t="s">
         <v>203</v>
@@ -4462,7 +4462,7 @@
         <v>349</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E85" t="s">
         <v>350</v>
@@ -4482,7 +4482,7 @@
         <v>202</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E86" t="s">
         <v>203</v>
@@ -4587,7 +4587,7 @@
         <v>349</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E92" t="s">
         <v>350</v>
@@ -4604,7 +4604,7 @@
         <v>202</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E93" t="s">
         <v>203</v>
@@ -4689,7 +4689,7 @@
         <v>354</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E98" t="s">
         <v>355</v>
@@ -4706,7 +4706,7 @@
         <v>202</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E99" t="s">
         <v>203</v>
@@ -4723,7 +4723,7 @@
         <v>358</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E100" t="s">
         <v>359</v>
@@ -4740,7 +4740,7 @@
         <v>361</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E101" t="s">
         <v>362</v>
@@ -4757,7 +4757,7 @@
         <v>364</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E102" t="s">
         <v>365</v>
@@ -4774,7 +4774,7 @@
         <v>367</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E103" t="s">
         <v>368</v>
@@ -4791,7 +4791,7 @@
         <v>370</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E104" t="s">
         <v>371</v>
@@ -4808,7 +4808,7 @@
         <v>373</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E105" t="s">
         <v>374</v>
@@ -4825,7 +4825,7 @@
         <v>376</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E106" t="s">
         <v>302</v>
@@ -4842,7 +4842,7 @@
         <v>202</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E107" t="s">
         <v>203</v>
@@ -4859,7 +4859,7 @@
         <v>219</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E108" t="s">
         <v>248</v>
@@ -4876,7 +4876,7 @@
         <v>221</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E109" t="s">
         <v>221</v>
@@ -4893,7 +4893,7 @@
         <v>202</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E110" t="s">
         <v>203</v>
@@ -4910,7 +4910,7 @@
         <v>380</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E111" t="s">
         <v>381</v>
@@ -4927,7 +4927,7 @@
         <v>383</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E112" t="s">
         <v>384</v>
@@ -4944,7 +4944,7 @@
         <v>386</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E113" t="s">
         <v>387</v>
@@ -4961,7 +4961,7 @@
         <v>202</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E114" t="s">
         <v>388</v>
@@ -4978,7 +4978,7 @@
         <v>219</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E115" t="s">
         <v>248</v>
@@ -4995,7 +4995,7 @@
         <v>221</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E116" t="s">
         <v>221</v>
@@ -5012,7 +5012,7 @@
         <v>202</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E117" t="s">
         <v>388</v>
@@ -5029,7 +5029,7 @@
         <v>392</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E118" t="s">
         <v>393</v>
@@ -5046,7 +5046,7 @@
         <v>395</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E119" t="s">
         <v>396</v>
@@ -5063,7 +5063,7 @@
         <v>202</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E120" t="s">
         <v>388</v>
@@ -5080,7 +5080,7 @@
         <v>399</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E121" t="s">
         <v>400</v>
@@ -5097,7 +5097,7 @@
         <v>402</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E122" t="s">
         <v>403</v>
@@ -5114,7 +5114,7 @@
         <v>405</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E123" t="s">
         <v>406</v>
@@ -5131,7 +5131,7 @@
         <v>408</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E124" t="s">
         <v>409</v>
@@ -5148,7 +5148,7 @@
         <v>215</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E125" t="s">
         <v>216</v>
@@ -5165,7 +5165,7 @@
         <v>202</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E126" t="s">
         <v>388</v>
@@ -5182,7 +5182,7 @@
         <v>219</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E127" t="s">
         <v>248</v>
@@ -5199,7 +5199,7 @@
         <v>221</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E128" t="s">
         <v>221</v>
@@ -5216,7 +5216,7 @@
         <v>202</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E129" t="s">
         <v>388</v>
@@ -5233,7 +5233,7 @@
         <v>219</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E130" t="s">
         <v>248</v>
@@ -5250,7 +5250,7 @@
         <v>221</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E131" t="s">
         <v>221</v>
@@ -5267,7 +5267,7 @@
         <v>202</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E132" t="s">
         <v>388</v>
@@ -5420,7 +5420,7 @@
         <v>202</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E141" t="s">
         <v>388</v>
@@ -5437,7 +5437,7 @@
         <v>415</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E142" t="s">
         <v>416</v>
@@ -5454,7 +5454,7 @@
         <v>418</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E143" t="s">
         <v>419</v>
@@ -5471,7 +5471,7 @@
         <v>421</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E144" t="s">
         <v>422</v>
@@ -5488,7 +5488,7 @@
         <v>424</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E145" t="s">
         <v>425</v>
@@ -5505,7 +5505,7 @@
         <v>427</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E146" t="s">
         <v>428</v>
@@ -5522,7 +5522,7 @@
         <v>430</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E147" t="s">
         <v>431</v>
@@ -5539,7 +5539,7 @@
         <v>433</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E148" t="s">
         <v>434</v>
@@ -5556,7 +5556,7 @@
         <v>202</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E149" t="s">
         <v>203</v>

</xml_diff>